<commit_message>
RAG, DIV#0 parameter added
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23451" windowHeight="10954" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23451" windowHeight="10954" tabRatio="587" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
-    <sheet name="Diagramme" sheetId="5" r:id="rId2"/>
-    <sheet name="Budgetierte Kosten" sheetId="1" r:id="rId3"/>
-    <sheet name="Tatsächliche Kosten" sheetId="2" r:id="rId4"/>
-    <sheet name="Fertigstellungsgrad der Akt." sheetId="3" r:id="rId5"/>
+    <sheet name="RAG" sheetId="6" r:id="rId2"/>
+    <sheet name="Diagramme" sheetId="5" r:id="rId3"/>
+    <sheet name="Budgetierte Kosten" sheetId="1" r:id="rId4"/>
+    <sheet name="Tatsächliche Kosten" sheetId="2" r:id="rId5"/>
+    <sheet name="Fertigstellungsgrad der Akt." sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="69">
   <si>
     <t>Aktivität / Monat</t>
   </si>
@@ -155,6 +156,81 @@
   </si>
   <si>
     <t>Baseline</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>Abgeschlossen</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Trend</t>
+  </si>
+  <si>
+    <t>Budget [k €]</t>
+  </si>
+  <si>
+    <t>Rot Grenze</t>
+  </si>
+  <si>
+    <t>Grün Grenze</t>
+  </si>
+  <si>
+    <t>Rot Text</t>
+  </si>
+  <si>
+    <t>Rot</t>
+  </si>
+  <si>
+    <t>Gelb Text</t>
+  </si>
+  <si>
+    <t>Gelb</t>
+  </si>
+  <si>
+    <t>Grün Text</t>
+  </si>
+  <si>
+    <t>Grün</t>
+  </si>
+  <si>
+    <t>Stand Monat 7</t>
+  </si>
+  <si>
+    <t>Stand Monat 6</t>
+  </si>
+  <si>
+    <t>Aufsteigender Trend</t>
+  </si>
+  <si>
+    <t>Abfallender Trend</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>NEG</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>Gleichbleibend</t>
+  </si>
+  <si>
+    <t>DIV#0</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Gleichbleibend Epsilon</t>
   </si>
 </sst>
 </file>
@@ -388,7 +464,7 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -419,6 +495,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent" xfId="13"/>
@@ -439,7 +520,10 @@
     <cellStyle name="Text" xfId="4"/>
     <cellStyle name="Warning" xfId="11"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="77">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -469,6 +553,234 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDE75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF49078"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDE75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF49078"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF49078"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -612,13 +924,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="SpBC" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="SpBC" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="37"/>
-      <tableStyleElement type="headerRow" dxfId="36"/>
-      <tableStyleElement type="totalRow" dxfId="35"/>
-      <tableStyleElement type="firstColumn" dxfId="34"/>
-      <tableStyleElement type="lastColumn" dxfId="33"/>
-      <tableStyleElement type="firstRowStripe" dxfId="32"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="31"/>
+      <tableStyleElement type="wholeTable" dxfId="76"/>
+      <tableStyleElement type="headerRow" dxfId="75"/>
+      <tableStyleElement type="totalRow" dxfId="74"/>
+      <tableStyleElement type="firstColumn" dxfId="73"/>
+      <tableStyleElement type="lastColumn" dxfId="72"/>
+      <tableStyleElement type="firstRowStripe" dxfId="71"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="70"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -689,6 +1001,13 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFF6969"/>
+      <color rgb="FFFF9797"/>
+      <color rgb="FFFF3300"/>
+      <color rgb="FFF56859"/>
+      <color rgb="FFFFDE75"/>
+      <color rgb="FFF49078"/>
+      <color rgb="FFED502B"/>
       <color rgb="FFF0F3FA"/>
       <color rgb="FFF6F8FC"/>
     </mruColors>
@@ -17969,29 +18288,57 @@
   </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" name="Posten"/>
-    <tableColumn id="2" name="1" dataDxfId="30">
+    <tableColumn id="2" name="1" dataDxfId="69">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!B2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="29">
+    <tableColumn id="3" name="2" dataDxfId="68">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!C2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" dataDxfId="28">
+    <tableColumn id="4" name="3" dataDxfId="67">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!D2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" dataDxfId="27">
+    <tableColumn id="5" name="4" dataDxfId="66">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!E2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" dataDxfId="26">
+    <tableColumn id="6" name="5" dataDxfId="65">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!F2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" dataDxfId="25">
+    <tableColumn id="7" name="6" dataDxfId="64">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!G2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="24">
+    <tableColumn id="8" name="7" dataDxfId="63">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!H2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabelle911" displayName="Tabelle911" ref="B17:H24" totalsRowShown="0">
+  <autoFilter ref="B17:H24"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Posten">
+      <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="CPI" dataDxfId="33">
+      <calculatedColumnFormula>Kennzahlen!H69</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="SPI" dataDxfId="32">
+      <calculatedColumnFormula>Kennzahlen!H82</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="19">
+      <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="35">
+      <calculatedColumnFormula>Kennzahlen!H4/1000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Status" dataDxfId="34">
+      <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Trend"/>
+  </tableColumns>
+  <tableStyleInfo name="SpBC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -18011,7 +18358,7 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="23">
+    <tableColumn id="2" name="1" dataDxfId="62">
       <calculatedColumnFormula>C4*'Fertigstellungsgrad der Akt.'!B2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -18053,15 +18400,15 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="22">
+    <tableColumn id="2" name="1" dataDxfId="61">
       <calculatedColumnFormula>'Tatsächliche Kosten'!B2*'Tatsächliche Kosten'!$B$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="21"/>
-    <tableColumn id="4" name="3" dataDxfId="20"/>
-    <tableColumn id="5" name="4" dataDxfId="19"/>
-    <tableColumn id="6" name="5" dataDxfId="18"/>
-    <tableColumn id="7" name="6" dataDxfId="17"/>
-    <tableColumn id="8" name="7" dataDxfId="16"/>
+    <tableColumn id="3" name="2" dataDxfId="60"/>
+    <tableColumn id="4" name="3" dataDxfId="59"/>
+    <tableColumn id="5" name="4" dataDxfId="58"/>
+    <tableColumn id="6" name="5" dataDxfId="57"/>
+    <tableColumn id="7" name="6" dataDxfId="56"/>
+    <tableColumn id="8" name="7" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18083,7 +18430,7 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="15">
+    <tableColumn id="2" name="1" dataDxfId="54">
       <calculatedColumnFormula>C30-C17</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -18116,7 +18463,7 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B43</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="14">
+    <tableColumn id="2" name="1" dataDxfId="53">
       <calculatedColumnFormula>C30-C4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -18149,25 +18496,25 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="7">
-      <calculatedColumnFormula>IF(C17=0,"-",C30/C17)</calculatedColumnFormula>
+    <tableColumn id="2" name="1" dataDxfId="12">
+      <calculatedColumnFormula>IF(C17=0,$L$70,C30/C17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="13">
-      <calculatedColumnFormula>IF(D17=0,"-",D30/D17)</calculatedColumnFormula>
+    <tableColumn id="3" name="2" dataDxfId="11">
+      <calculatedColumnFormula>IF(D17=0,$L$70,D30/D17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" dataDxfId="12">
-      <calculatedColumnFormula>IF(E17=0,"-",E30/E17)</calculatedColumnFormula>
+    <tableColumn id="4" name="3" dataDxfId="10">
+      <calculatedColumnFormula>IF(E17=0,$L$70,E30/E17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" dataDxfId="11">
-      <calculatedColumnFormula>IF(F17=0,"-",F30/F17)</calculatedColumnFormula>
+    <tableColumn id="5" name="4" dataDxfId="9">
+      <calculatedColumnFormula>IF(F17=0,$L$70,F30/F17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" dataDxfId="10">
-      <calculatedColumnFormula>IF(G17=0,"-",G30/G17)</calculatedColumnFormula>
+    <tableColumn id="6" name="5" dataDxfId="8">
+      <calculatedColumnFormula>IF(G17=0,$L$70,G30/G17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" dataDxfId="9">
-      <calculatedColumnFormula>IF(H17=0,"-",H30/H17)</calculatedColumnFormula>
+    <tableColumn id="7" name="6" dataDxfId="7">
+      <calculatedColumnFormula>IF(H17=0,$L$70,H30/H17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="8">
+    <tableColumn id="8" name="7" dataDxfId="52">
       <calculatedColumnFormula>IF(I17=0,"-",I30/I17)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18183,24 +18530,24 @@
       <calculatedColumnFormula>B69</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="1" dataDxfId="6">
-      <calculatedColumnFormula>IF(C4=0,"-",C30/C4)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(C4=0,$L$70,C30/C4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2" dataDxfId="5">
-      <calculatedColumnFormula>IF(D4=0,"-",D30/D4)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(D4=0,$L$70,D30/D4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="3" dataDxfId="4">
-      <calculatedColumnFormula>IF(E4=0,"-",E30/E4)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(E4=0,$L$70,E30/E4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="4" dataDxfId="3">
-      <calculatedColumnFormula>IF(F4=0,"-",F30/F4)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(F4=0,$L$70,F30/F4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="5" dataDxfId="2">
-      <calculatedColumnFormula>IF(G4=0,"-",G30/G4)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(G4=0,$L$70,G30/G4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="6" dataDxfId="1">
-      <calculatedColumnFormula>IF(H4=0,"-",H30/H4)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(H4=0,$L$70,H30/H4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="0">
+    <tableColumn id="8" name="7" dataDxfId="51">
       <calculatedColumnFormula>IF(I4=0,"-",I30/I4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18219,6 +18566,34 @@
     <tableColumn id="6" name="5"/>
     <tableColumn id="7" name="6"/>
     <tableColumn id="8" name="7"/>
+  </tableColumns>
+  <tableStyleInfo name="SpBC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabelle9" displayName="Tabelle9" ref="B4:H11" totalsRowShown="0">
+  <autoFilter ref="B4:H11"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Posten">
+      <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="CPI" dataDxfId="50">
+      <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="SPI" dataDxfId="49">
+      <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="48">
+      <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="47"/>
+    <tableColumn id="6" name="Status" dataDxfId="45">
+      <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Trend" dataDxfId="0">
+      <calculatedColumnFormula>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18608,8 +18983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T88"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="S72" sqref="S72"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -20059,31 +20434,31 @@
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C69" s="29">
-        <f t="shared" ref="C69:I69" si="18">IF(C17=0,"-",C30/C17)</f>
+        <f t="shared" ref="C69:C75" si="18">IF(C17=0,$L$70,C30/C17)</f>
         <v>0.3952941176470588</v>
       </c>
       <c r="D69" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="D69:D75" si="19">IF(D17=0,$L$70,D30/D17)</f>
         <v>5.647058823529412E-2</v>
       </c>
       <c r="E69" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="E69:E75" si="20">IF(E17=0,$L$70,E30/E17)</f>
         <v>0.11000763941940413</v>
       </c>
       <c r="F69" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="F69:F75" si="21">IF(F17=0,$L$70,F30/F17)</f>
         <v>0.31964483906770258</v>
       </c>
       <c r="G69" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="G69:G75" si="22">IF(G17=0,$L$70,G30/G17)</f>
         <v>0.53274139844617097</v>
       </c>
       <c r="H69" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="H69:H75" si="23">IF(H17=0,$L$70,H30/H17)</f>
         <v>0.85238623751387343</v>
       </c>
       <c r="I69" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="C69:I69" si="24">IF(I17=0,"-",I30/I17)</f>
         <v>0.95893451720310763</v>
       </c>
       <c r="K69" t="s">
@@ -20119,15 +20494,15 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B70" t="str">
-        <f t="shared" ref="B70:B74" si="19">B57</f>
+        <f t="shared" ref="B70:B74" si="25">B57</f>
         <v>Design und Architektur</v>
       </c>
       <c r="C70" s="29" t="str">
-        <f t="shared" ref="C70:I70" si="20">IF(C18=0,"-",C31/C18)</f>
+        <f t="shared" si="18"/>
         <v>-</v>
       </c>
       <c r="D70" s="29" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>-</v>
       </c>
       <c r="E70" s="29" t="str">
@@ -20135,37 +20510,43 @@
         <v>-</v>
       </c>
       <c r="F70" s="29">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.1176470588235297E-2</v>
       </c>
       <c r="G70" s="29">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.067226890756303E-2</v>
       </c>
       <c r="H70" s="29">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.19228336495888679</v>
       </c>
       <c r="I70" s="29">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="C70:I70" si="26">IF(I18=0,"-",I31/I18)</f>
         <v>0.78583666476299252</v>
+      </c>
+      <c r="K70" t="s">
+        <v>66</v>
+      </c>
+      <c r="L70" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B71" t="str">
+        <f t="shared" si="25"/>
+        <v>Implementierung</v>
+      </c>
+      <c r="C71" s="29" t="str">
+        <f t="shared" si="18"/>
+        <v>-</v>
+      </c>
+      <c r="D71" s="29" t="str">
         <f t="shared" si="19"/>
-        <v>Implementierung</v>
-      </c>
-      <c r="C71" s="29" t="str">
-        <f t="shared" ref="C71:I71" si="21">IF(C19=0,"-",C32/C19)</f>
         <v>-</v>
       </c>
-      <c r="D71" s="29" t="str">
-        <f t="shared" si="21"/>
-        <v>-</v>
-      </c>
       <c r="E71" s="29" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>-</v>
       </c>
       <c r="F71" s="29" t="str">
@@ -20173,37 +20554,37 @@
         <v>-</v>
       </c>
       <c r="G71" s="29" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>-</v>
       </c>
       <c r="H71" s="29">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.5270588235294118</v>
       </c>
       <c r="I71" s="29">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="C71:I71" si="27">IF(I19=0,"-",I32/I19)</f>
         <v>0.94117647058823528</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B72" t="str">
+        <f t="shared" si="25"/>
+        <v>Integration und Test</v>
+      </c>
+      <c r="C72" s="29" t="str">
+        <f t="shared" si="18"/>
+        <v>-</v>
+      </c>
+      <c r="D72" s="29" t="str">
         <f t="shared" si="19"/>
-        <v>Integration und Test</v>
-      </c>
-      <c r="C72" s="29" t="str">
-        <f t="shared" ref="C72:I72" si="22">IF(C20=0,"-",C33/C20)</f>
         <v>-</v>
       </c>
-      <c r="D72" s="29" t="str">
-        <f t="shared" si="22"/>
+      <c r="E72" s="29" t="str">
+        <f t="shared" si="20"/>
         <v>-</v>
       </c>
-      <c r="E72" s="29" t="str">
-        <f t="shared" si="22"/>
-        <v>-</v>
-      </c>
       <c r="F72" s="29" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>-</v>
       </c>
       <c r="G72" s="29" t="str">
@@ -20211,37 +20592,37 @@
         <v>-</v>
       </c>
       <c r="H72" s="29" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>-</v>
       </c>
       <c r="I72" s="29">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="C72:I72" si="28">IF(I20=0,"-",I33/I20)</f>
         <v>0.13445378151260504</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B73" t="str">
+        <f t="shared" si="25"/>
+        <v>Projektmanagement</v>
+      </c>
+      <c r="C73" s="29">
+        <f t="shared" si="18"/>
+        <v>6.9019607843137251E-2</v>
+      </c>
+      <c r="D73" s="29">
         <f t="shared" si="19"/>
-        <v>Projektmanagement</v>
-      </c>
-      <c r="C73" s="29">
-        <f t="shared" ref="C73:I73" si="23">IF(C21=0,"-",C34/C21)</f>
-        <v>6.9019607843137251E-2</v>
-      </c>
-      <c r="D73" s="29">
-        <f t="shared" si="23"/>
         <v>2.3529411764705882E-2</v>
       </c>
       <c r="E73" s="29">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>7.7647058823529416E-2</v>
       </c>
       <c r="F73" s="29">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11503267973856209</v>
       </c>
       <c r="G73" s="29">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.19411764705882353</v>
       </c>
       <c r="H73" s="29">
@@ -20249,41 +20630,41 @@
         <v>0.28235294117647058</v>
       </c>
       <c r="I73" s="29">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="C73:I73" si="29">IF(I21=0,"-",I34/I21)</f>
         <v>0.37745098039215685</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B74" t="str">
+        <f t="shared" si="25"/>
+        <v>Puffer für unerwartetes</v>
+      </c>
+      <c r="C74" s="29">
+        <f t="shared" si="18"/>
+        <v>4.7058823529411764E-2</v>
+      </c>
+      <c r="D74" s="29">
         <f t="shared" si="19"/>
-        <v>Puffer für unerwartetes</v>
-      </c>
-      <c r="C74" s="29">
-        <f t="shared" ref="C74:I74" si="24">IF(C22=0,"-",C35/C22)</f>
-        <v>4.7058823529411764E-2</v>
-      </c>
-      <c r="D74" s="29">
-        <f t="shared" si="24"/>
         <v>4.8019207683073226E-3</v>
       </c>
       <c r="E74" s="29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>7.9312623925974889E-3</v>
       </c>
       <c r="F74" s="29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>1.8776587941909929E-2</v>
       </c>
       <c r="G74" s="29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>3.4772529701535784E-2</v>
       </c>
       <c r="H74" s="29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>6.1829111206526406E-2</v>
       </c>
       <c r="I74" s="29">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="C74:I74" si="30">IF(I22=0,"-",I35/I22)</f>
         <v>8.7104072398190055E-2</v>
       </c>
     </row>
@@ -20293,27 +20674,27 @@
         <v>Materialkosten</v>
       </c>
       <c r="C75" s="29">
-        <f t="shared" ref="C75:H75" si="25">IF(C23=0,"-",C36/C23)</f>
+        <f t="shared" si="18"/>
         <v>0.02</v>
       </c>
       <c r="D75" s="29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>4.5714285714285714E-2</v>
       </c>
       <c r="E75" s="29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>8.5714285714285715E-2</v>
       </c>
       <c r="F75" s="29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0.125</v>
       </c>
       <c r="G75" s="29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>0.17567567567567569</v>
       </c>
       <c r="H75" s="29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.128</v>
       </c>
       <c r="I75" s="29">
@@ -20358,31 +20739,31 @@
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C82" s="29">
-        <f t="shared" ref="C82:I82" si="26">IF(C4=0,"-",C30/C4)</f>
+        <f t="shared" ref="C82:C88" si="31">IF(C4=0,$L$70,C30/C4)</f>
         <v>0.35</v>
       </c>
       <c r="D82" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="D82:D88" si="32">IF(D4=0,$L$70,D30/D4)</f>
         <v>0.05</v>
       </c>
       <c r="E82" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="E82:E88" si="33">IF(E4=0,$L$70,E30/E4)</f>
         <v>0.1</v>
       </c>
       <c r="F82" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="F82:F88" si="34">IF(F4=0,$L$70,F30/F4)</f>
         <v>0.3</v>
       </c>
       <c r="G82" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="G82:G88" si="35">IF(G4=0,$L$70,G30/G4)</f>
         <v>0.5</v>
       </c>
       <c r="H82" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="H82:H88" si="36">IF(H4=0,$L$70,H30/H4)</f>
         <v>0.8</v>
       </c>
       <c r="I82" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="C82:I82" si="37">IF(I4=0,"-",I30/I4)</f>
         <v>0.9</v>
       </c>
       <c r="K82" t="s">
@@ -20397,147 +20778,147 @@
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B83" t="str">
-        <f t="shared" ref="B83:B87" si="27">B70</f>
+        <f t="shared" ref="B83:B87" si="38">B70</f>
         <v>Design und Architektur</v>
       </c>
       <c r="C83" s="29" t="str">
-        <f t="shared" ref="C83:I83" si="28">IF(C5=0,"-",C31/C5)</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="D83" s="29" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>-</v>
       </c>
       <c r="E83" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="F83" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0.05</v>
       </c>
       <c r="G83" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>0.05</v>
       </c>
       <c r="H83" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0.1</v>
       </c>
       <c r="I83" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="C83:I83" si="39">IF(I5=0,"-",I31/I5)</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="84" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B84" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="38"/>
         <v>Implementierung</v>
       </c>
       <c r="C84" s="29" t="str">
-        <f t="shared" ref="C84:I84" si="29">IF(C6=0,"-",C32/C6)</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="D84" s="29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>-</v>
       </c>
       <c r="E84" s="29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-</v>
       </c>
       <c r="F84" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="G84" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="H84" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.1</v>
       </c>
       <c r="I84" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="C84:I84" si="40">IF(I6=0,"-",I32/I6)</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B85" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="38"/>
         <v>Integration und Test</v>
       </c>
       <c r="C85" s="29" t="str">
-        <f t="shared" ref="C85:I85" si="30">IF(C7=0,"-",C33/C7)</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="D85" s="29" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-</v>
       </c>
       <c r="E85" s="29" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>-</v>
       </c>
       <c r="F85" s="29" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>-</v>
       </c>
       <c r="G85" s="29" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>-</v>
       </c>
       <c r="H85" s="29" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>-</v>
       </c>
       <c r="I85" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="C85:I85" si="41">IF(I7=0,"-",I33/I7)</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="86" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B86" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="38"/>
         <v>Projektmanagement</v>
       </c>
       <c r="C86" s="29">
-        <f t="shared" ref="C86:I86" si="31">IF(C8=0,"-",C34/C8)</f>
+        <f t="shared" si="31"/>
         <v>0.08</v>
       </c>
       <c r="D86" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.05</v>
       </c>
       <c r="E86" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.15</v>
       </c>
       <c r="F86" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="G86" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>0.3</v>
       </c>
       <c r="H86" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>0.4</v>
       </c>
       <c r="I86" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="C86:I86" si="42">IF(I8=0,"-",I34/I8)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="87" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B87" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="38"/>
         <v>Puffer für unerwartetes</v>
       </c>
       <c r="C87" s="29">
-        <f t="shared" ref="C87:I87" si="32">IF(C9=0,"-",C35/C9)</f>
+        <f t="shared" si="31"/>
         <v>0.08</v>
       </c>
       <c r="D87" s="29">
@@ -20545,23 +20926,23 @@
         <v>0.05</v>
       </c>
       <c r="E87" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.1</v>
       </c>
       <c r="F87" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="G87" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.3</v>
       </c>
       <c r="H87" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0.45</v>
       </c>
       <c r="I87" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="C87:I87" si="43">IF(I9=0,"-",I35/I9)</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -20571,11 +20952,11 @@
         <v>Materialkosten</v>
       </c>
       <c r="C88" s="29">
-        <f t="shared" ref="C88:I88" si="33">IF(C10=0,"-",C36/C10)</f>
+        <f t="shared" si="31"/>
         <v>0.02</v>
       </c>
       <c r="D88" s="29">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.04</v>
       </c>
       <c r="E88" s="29">
@@ -20583,19 +20964,19 @@
         <v>0.06</v>
       </c>
       <c r="F88" s="29">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.08</v>
       </c>
       <c r="G88" s="29">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.1</v>
       </c>
       <c r="H88" s="29">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0.12</v>
       </c>
       <c r="I88" s="29">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="C88:I88" si="44">IF(I10=0,"-",I36/I10)</f>
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -20617,10 +20998,598 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.23046875" customWidth="1"/>
+    <col min="5" max="5" width="16.07421875" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.4609375" customWidth="1"/>
+    <col min="10" max="10" width="18.3828125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="22.3" x14ac:dyDescent="0.5">
+      <c r="A2" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="str">
+        <f>Kennzahlen!B56</f>
+        <v>Anforderungsanalyse</v>
+      </c>
+      <c r="C5" s="29">
+        <f>Kennzahlen!I69</f>
+        <v>0.95893451720310763</v>
+      </c>
+      <c r="D5" s="29">
+        <f>Kennzahlen!I82</f>
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!H2</f>
+        <v>0.9</v>
+      </c>
+      <c r="F5" s="31">
+        <f>'Budgetierte Kosten'!P2/1000</f>
+        <v>144</v>
+      </c>
+      <c r="G5" s="32" t="str">
+        <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Gelb</v>
+      </c>
+      <c r="H5" t="str">
+        <f>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</f>
+        <v>POS</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="str">
+        <f>Kennzahlen!B57</f>
+        <v>Design und Architektur</v>
+      </c>
+      <c r="C6" s="29">
+        <f>Kennzahlen!I70</f>
+        <v>0.78583666476299252</v>
+      </c>
+      <c r="D6" s="29">
+        <f>Kennzahlen!I83</f>
+        <v>0.4</v>
+      </c>
+      <c r="E6" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!H3</f>
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="31">
+        <f>'Budgetierte Kosten'!P3/1000</f>
+        <v>236</v>
+      </c>
+      <c r="G6" s="32" t="str">
+        <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+      <c r="H6" t="str">
+        <f>IF(C19=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C19)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C19,Tabelle9[[#This Row],[SPI]]&lt;D19), $K$11, $K$10)))</f>
+        <v>POS</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="str">
+        <f>Kennzahlen!B58</f>
+        <v>Implementierung</v>
+      </c>
+      <c r="C7" s="29">
+        <f>Kennzahlen!I71</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="D7" s="29">
+        <f>Kennzahlen!I84</f>
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!H4</f>
+        <v>0.25</v>
+      </c>
+      <c r="F7" s="31">
+        <f>'Budgetierte Kosten'!P4/1000</f>
+        <v>392</v>
+      </c>
+      <c r="G7" s="32" t="str">
+        <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+      <c r="H7" t="str">
+        <f>IF(C20=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C20)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C20,Tabelle9[[#This Row],[SPI]]&lt;D20), $K$11, $K$10)))</f>
+        <v>POS</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="str">
+        <f>Kennzahlen!B59</f>
+        <v>Integration und Test</v>
+      </c>
+      <c r="C8" s="29">
+        <f>Kennzahlen!I72</f>
+        <v>0.13445378151260504</v>
+      </c>
+      <c r="D8" s="29">
+        <f>Kennzahlen!I85</f>
+        <v>0.25</v>
+      </c>
+      <c r="E8" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!H5</f>
+        <v>0.25</v>
+      </c>
+      <c r="F8" s="31">
+        <f>'Budgetierte Kosten'!P5/1000</f>
+        <v>252</v>
+      </c>
+      <c r="G8" s="32" t="str">
+        <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+      <c r="H8" t="str">
+        <f>IF(C21=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C21)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C21,Tabelle9[[#This Row],[SPI]]&lt;D21), $K$11, $K$10)))</f>
+        <v>-</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B9" t="str">
+        <f>Kennzahlen!B60</f>
+        <v>Projektmanagement</v>
+      </c>
+      <c r="C9" s="29">
+        <f>Kennzahlen!I73</f>
+        <v>0.37745098039215685</v>
+      </c>
+      <c r="D9" s="29">
+        <f>Kennzahlen!I86</f>
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!H6</f>
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="31">
+        <f>'Budgetierte Kosten'!P6/1000</f>
+        <v>286</v>
+      </c>
+      <c r="G9" s="32" t="str">
+        <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+      <c r="H9" t="str">
+        <f>IF(C22=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C22)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C22,Tabelle9[[#This Row],[SPI]]&lt;D22), $K$11, $K$10)))</f>
+        <v>POS</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="str">
+        <f>Kennzahlen!B61</f>
+        <v>Puffer für unerwartetes</v>
+      </c>
+      <c r="C10" s="29">
+        <f>Kennzahlen!I74</f>
+        <v>8.7104072398190055E-2</v>
+      </c>
+      <c r="D10" s="29">
+        <f>Kennzahlen!I87</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E10" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!H7</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F10" s="31">
+        <f>'Budgetierte Kosten'!P7/1000</f>
+        <v>104</v>
+      </c>
+      <c r="G10" s="32" t="str">
+        <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+      <c r="H10" t="str">
+        <f>IF(C23=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C23)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C23,Tabelle9[[#This Row],[SPI]]&lt;D23), $K$11, $K$10)))</f>
+        <v>EQ</v>
+      </c>
+      <c r="J10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <f>Kennzahlen!B62</f>
+        <v>Materialkosten</v>
+      </c>
+      <c r="C11" s="29">
+        <f>Kennzahlen!I75</f>
+        <v>0.18148148148148152</v>
+      </c>
+      <c r="D11" s="29">
+        <f>Kennzahlen!I88</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E11" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!H8</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F11" s="31">
+        <f>'Budgetierte Kosten'!O11/1000</f>
+        <v>86</v>
+      </c>
+      <c r="G11" s="32" t="str">
+        <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+      <c r="H11" t="str">
+        <f>IF(C24=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C24)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C24,Tabelle9[[#This Row],[SPI]]&lt;D24), $K$11, $K$10)))</f>
+        <v>POS</v>
+      </c>
+      <c r="J11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="22.3" x14ac:dyDescent="0.5">
+      <c r="A15" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <f>Kennzahlen!B69</f>
+        <v>Anforderungsanalyse</v>
+      </c>
+      <c r="C18" s="29">
+        <f>Kennzahlen!H69</f>
+        <v>0.85238623751387343</v>
+      </c>
+      <c r="D18" s="29">
+        <f>Kennzahlen!H82</f>
+        <v>0.8</v>
+      </c>
+      <c r="E18" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!G2</f>
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="31">
+        <f>Kennzahlen!H4/1000</f>
+        <v>144</v>
+      </c>
+      <c r="G18" s="32" t="str">
+        <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Gelb</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <f>Kennzahlen!B70</f>
+        <v>Design und Architektur</v>
+      </c>
+      <c r="C19" s="29">
+        <f>Kennzahlen!H70</f>
+        <v>0.19228336495888679</v>
+      </c>
+      <c r="D19" s="29">
+        <f>Kennzahlen!H83</f>
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!G3</f>
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="31">
+        <f>Kennzahlen!H5/1000</f>
+        <v>152</v>
+      </c>
+      <c r="G19" s="32" t="str">
+        <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <f>Kennzahlen!B71</f>
+        <v>Implementierung</v>
+      </c>
+      <c r="C20" s="29">
+        <f>Kennzahlen!H71</f>
+        <v>0.5270588235294118</v>
+      </c>
+      <c r="D20" s="29">
+        <f>Kennzahlen!H84</f>
+        <v>0.1</v>
+      </c>
+      <c r="E20" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!G4</f>
+        <v>0.1</v>
+      </c>
+      <c r="F20" s="31">
+        <f>Kennzahlen!H6/1000</f>
+        <v>112</v>
+      </c>
+      <c r="G20" s="32" t="str">
+        <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <f>Kennzahlen!B72</f>
+        <v>Integration und Test</v>
+      </c>
+      <c r="C21" s="29" t="str">
+        <f>Kennzahlen!H72</f>
+        <v>-</v>
+      </c>
+      <c r="D21" s="29" t="str">
+        <f>Kennzahlen!H85</f>
+        <v>-</v>
+      </c>
+      <c r="E21" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!G5</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="31">
+        <f>Kennzahlen!H7/1000</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="32" t="str">
+        <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Grün</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <f>Kennzahlen!B73</f>
+        <v>Projektmanagement</v>
+      </c>
+      <c r="C22" s="29">
+        <f>Kennzahlen!H73</f>
+        <v>0.28235294117647058</v>
+      </c>
+      <c r="D22" s="29">
+        <f>Kennzahlen!H86</f>
+        <v>0.4</v>
+      </c>
+      <c r="E22" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!G6</f>
+        <v>0.4</v>
+      </c>
+      <c r="F22" s="31">
+        <f>Kennzahlen!H8/1000</f>
+        <v>132</v>
+      </c>
+      <c r="G22" s="32" t="str">
+        <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <f>Kennzahlen!B74</f>
+        <v>Puffer für unerwartetes</v>
+      </c>
+      <c r="C23" s="29">
+        <f>Kennzahlen!H74</f>
+        <v>6.1829111206526406E-2</v>
+      </c>
+      <c r="D23" s="29">
+        <f>Kennzahlen!H87</f>
+        <v>0.45</v>
+      </c>
+      <c r="E23" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!G7</f>
+        <v>0.45</v>
+      </c>
+      <c r="F23" s="31">
+        <f>Kennzahlen!H9/1000</f>
+        <v>48</v>
+      </c>
+      <c r="G23" s="32" t="str">
+        <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="str">
+        <f>Kennzahlen!B75</f>
+        <v>Materialkosten</v>
+      </c>
+      <c r="C24" s="29">
+        <f>Kennzahlen!H75</f>
+        <v>0.128</v>
+      </c>
+      <c r="D24" s="29">
+        <f>Kennzahlen!H88</f>
+        <v>0.12</v>
+      </c>
+      <c r="E24" s="30">
+        <f>'Fertigstellungsgrad der Akt.'!G8</f>
+        <v>0.12</v>
+      </c>
+      <c r="F24" s="31">
+        <f>Kennzahlen!H10/1000</f>
+        <v>16</v>
+      </c>
+      <c r="G24" s="32" t="str">
+        <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
+        <v>Rot</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C5:D11 C18:D24">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="greaterThanOrEqual">
+      <formula>$K$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="lessThan">
+      <formula>$K$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="lessThan">
+      <formula>$K$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{E0B5B186-BB25-4080-B948-EED301F00D0A}">
+            <xm:f>NOT(ISERROR(SEARCH($K$8,G5)))</xm:f>
+            <xm:f>$K$8</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{A789120A-4B68-43F8-9616-2D4E41C8BD80}">
+            <xm:f>NOT(ISERROR(SEARCH($K$7,G5)))</xm:f>
+            <xm:f>$K$7</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{531456C6-9606-47DB-9456-B0A7E2B1691B}">
+            <xm:f>NOT(ISERROR(SEARCH($K$6,G5)))</xm:f>
+            <xm:f>$K$6</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF6969"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G5:G11 G18:G24</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" zoomScale="51" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -20631,11 +21600,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -21296,7 +22265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
@@ -21672,7 +22641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>

</xml_diff>

<commit_message>
added EAC, ETC calculation
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sack\Christian\A\Studium\4 - Semester\SpBC\Übungen\swpbc\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Karriere\TU\2017SS\SwPBC\swpbc\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23451" windowHeight="10954" tabRatio="587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="75">
   <si>
     <t>Aktivität / Monat</t>
   </si>
@@ -149,9 +149,6 @@
     <t>EV / PV</t>
   </si>
   <si>
-    <t>EV / AV</t>
-  </si>
-  <si>
     <t>AC (Actual Cost)</t>
   </si>
   <si>
@@ -232,6 +229,27 @@
   <si>
     <t>Gleichbleibend Epsilon</t>
   </si>
+  <si>
+    <t>ETC (Estimate to complete)</t>
+  </si>
+  <si>
+    <t>(BAC - EV) / CPI</t>
+  </si>
+  <si>
+    <t>€</t>
+  </si>
+  <si>
+    <t>BAC (Budget at Completion)</t>
+  </si>
+  <si>
+    <t>EAC (Estimate at Completion)</t>
+  </si>
+  <si>
+    <t>BAC / CPI</t>
+  </si>
+  <si>
+    <t>EV / AC</t>
+  </si>
 </sst>
 </file>
 
@@ -244,7 +262,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -349,6 +367,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -464,7 +487,7 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -500,6 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent" xfId="13"/>
@@ -520,16 +544,12 @@
     <cellStyle name="Text" xfId="4"/>
     <cellStyle name="Warning" xfId="11"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="73">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -538,17 +558,10 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -597,6 +610,71 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -770,13 +848,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="SpBC" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="SpBC" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="54"/>
-      <tableStyleElement type="headerRow" dxfId="53"/>
-      <tableStyleElement type="totalRow" dxfId="52"/>
-      <tableStyleElement type="firstColumn" dxfId="51"/>
-      <tableStyleElement type="lastColumn" dxfId="50"/>
-      <tableStyleElement type="firstRowStripe" dxfId="49"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="48"/>
+      <tableStyleElement type="wholeTable" dxfId="72"/>
+      <tableStyleElement type="headerRow" dxfId="71"/>
+      <tableStyleElement type="totalRow" dxfId="70"/>
+      <tableStyleElement type="firstColumn" dxfId="69"/>
+      <tableStyleElement type="lastColumn" dxfId="68"/>
+      <tableStyleElement type="firstRowStripe" dxfId="67"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="66"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -4615,6 +4693,357 @@
           <c:h val="0.53144491760887669"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Anforderungsanalyse</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>ETC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Kennzahlen!$C$97:$I$97</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3119702.3809523811</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22050416.666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11231947.222222222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3775440.2777777775</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2211204.1666666665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1331321.3541666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1168380.0925925926</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8D7F-47F6-ACF8-67F3B6711F55}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="388250192"/>
+        <c:axId val="388253472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="388250192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388253472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="388253472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388250192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10041,6 +10470,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12942,6 +13411,522 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18117,6 +19102,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>543483</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>40341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>543483</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Diagramm 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC8165B6-1761-4DE5-B9E3-9DF72546127E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -18134,25 +19155,25 @@
   </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" name="Posten"/>
-    <tableColumn id="2" name="1" dataDxfId="47">
+    <tableColumn id="2" name="1" dataDxfId="65">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!B2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="46">
+    <tableColumn id="3" name="2" dataDxfId="64">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!C2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" dataDxfId="45">
+    <tableColumn id="4" name="3" dataDxfId="63">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!D2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" dataDxfId="44">
+    <tableColumn id="5" name="4" dataDxfId="62">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!E2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" dataDxfId="43">
+    <tableColumn id="6" name="5" dataDxfId="61">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!F2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" dataDxfId="42">
+    <tableColumn id="7" name="6" dataDxfId="60">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!G2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="41">
+    <tableColumn id="8" name="7" dataDxfId="59">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!H2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18161,25 +19182,86 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabelle46781213" displayName="Tabelle46781213" ref="B109:I116" totalsRowShown="0">
+  <autoFilter ref="B109:I116"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Posten" dataDxfId="1">
+      <calculatedColumnFormula>B97</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="1" dataDxfId="0">
+      <calculatedColumnFormula>IF(C69=$L$70,$L$70,$E$92/C69)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="2" dataDxfId="7">
+      <calculatedColumnFormula>IF(D69=$L$70,$L$70,$E$92/D69)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="3" dataDxfId="6">
+      <calculatedColumnFormula>IF(E69=$L$70,$L$70,$E$92/E69)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="4" dataDxfId="5">
+      <calculatedColumnFormula>IF(F69=$L$70,$L$70,$E$92/F69)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="5" dataDxfId="4">
+      <calculatedColumnFormula>IF(G69=$L$70,$L$70,$E$92/G69)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="6" dataDxfId="3">
+      <calculatedColumnFormula>IF(H69=$L$70,$L$70,$E$92/H69)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="7" dataDxfId="2">
+      <calculatedColumnFormula>IF(I69=$L$70,$L$70,$E$92/I69)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabelle9" displayName="Tabelle9" ref="B4:H11" totalsRowShown="0">
+  <autoFilter ref="B4:H11"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Posten">
+      <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="CPI" dataDxfId="34">
+      <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="SPI" dataDxfId="33">
+      <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="32">
+      <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="31"/>
+    <tableColumn id="6" name="Status" dataDxfId="30">
+      <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Trend" dataDxfId="29">
+      <calculatedColumnFormula>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="SpBC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabelle911" displayName="Tabelle911" ref="B17:H24" totalsRowShown="0">
   <autoFilter ref="B17:H24"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="4">
+    <tableColumn id="2" name="CPI" dataDxfId="28">
       <calculatedColumnFormula>Kennzahlen!H69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="3">
+    <tableColumn id="3" name="SPI" dataDxfId="27">
       <calculatedColumnFormula>Kennzahlen!H82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="2">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="26">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="1">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="25">
       <calculatedColumnFormula>Kennzahlen!H4/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Status" dataDxfId="0">
+    <tableColumn id="6" name="Status" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Trend"/>
@@ -18201,10 +19283,10 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" name="Posten">
-      <calculatedColumnFormula>B4</calculatedColumnFormula>
+    <tableColumn id="1" name="Posten" dataDxfId="22">
+      <calculatedColumnFormula>B17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="40">
+    <tableColumn id="2" name="1" dataDxfId="58">
       <calculatedColumnFormula>C4*'Fertigstellungsgrad der Akt.'!B2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -18243,18 +19325,18 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" name="Posten">
+    <tableColumn id="1" name="Posten" dataDxfId="23">
       <calculatedColumnFormula>B4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="39">
+    <tableColumn id="2" name="1" dataDxfId="57">
       <calculatedColumnFormula>'Tatsächliche Kosten'!B2*'Tatsächliche Kosten'!$B$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="38"/>
-    <tableColumn id="4" name="3" dataDxfId="37"/>
-    <tableColumn id="5" name="4" dataDxfId="36"/>
-    <tableColumn id="6" name="5" dataDxfId="35"/>
-    <tableColumn id="7" name="6" dataDxfId="34"/>
-    <tableColumn id="8" name="7" dataDxfId="33"/>
+    <tableColumn id="3" name="2" dataDxfId="56"/>
+    <tableColumn id="4" name="3" dataDxfId="55"/>
+    <tableColumn id="5" name="4" dataDxfId="54"/>
+    <tableColumn id="6" name="5" dataDxfId="53"/>
+    <tableColumn id="7" name="6" dataDxfId="52"/>
+    <tableColumn id="8" name="7" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18276,7 +19358,7 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="32">
+    <tableColumn id="2" name="1" dataDxfId="50">
       <calculatedColumnFormula>C30-C17</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -18309,7 +19391,7 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B43</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="31">
+    <tableColumn id="2" name="1" dataDxfId="49">
       <calculatedColumnFormula>C30-C4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -18342,25 +19424,25 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="30">
+    <tableColumn id="2" name="1" dataDxfId="48">
       <calculatedColumnFormula>IF(C17=0,$L$70,C30/C17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="29">
+    <tableColumn id="3" name="2" dataDxfId="47">
       <calculatedColumnFormula>IF(D17=0,$L$70,D30/D17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" dataDxfId="28">
+    <tableColumn id="4" name="3" dataDxfId="46">
       <calculatedColumnFormula>IF(E17=0,$L$70,E30/E17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" dataDxfId="27">
+    <tableColumn id="5" name="4" dataDxfId="45">
       <calculatedColumnFormula>IF(F17=0,$L$70,F30/F17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" dataDxfId="26">
+    <tableColumn id="6" name="5" dataDxfId="44">
       <calculatedColumnFormula>IF(G17=0,$L$70,G30/G17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" dataDxfId="25">
+    <tableColumn id="7" name="6" dataDxfId="43">
       <calculatedColumnFormula>IF(H17=0,$L$70,H30/H17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="24">
+    <tableColumn id="8" name="7" dataDxfId="42">
       <calculatedColumnFormula>IF(I17=0,"-",I30/I17)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18375,25 +19457,25 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="23">
+    <tableColumn id="2" name="1" dataDxfId="41">
       <calculatedColumnFormula>IF(C4=0,$L$70,C30/C4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="22">
+    <tableColumn id="3" name="2" dataDxfId="40">
       <calculatedColumnFormula>IF(D4=0,$L$70,D30/D4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" dataDxfId="21">
+    <tableColumn id="4" name="3" dataDxfId="39">
       <calculatedColumnFormula>IF(E4=0,$L$70,E30/E4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" dataDxfId="20">
+    <tableColumn id="5" name="4" dataDxfId="38">
       <calculatedColumnFormula>IF(F4=0,$L$70,F30/F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" dataDxfId="19">
+    <tableColumn id="6" name="5" dataDxfId="37">
       <calculatedColumnFormula>IF(G4=0,$L$70,G30/G4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" dataDxfId="18">
+    <tableColumn id="7" name="6" dataDxfId="36">
       <calculatedColumnFormula>IF(H4=0,$L$70,H30/H4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="17">
+    <tableColumn id="8" name="7" dataDxfId="35">
       <calculatedColumnFormula>IF(I4=0,"-",I30/I4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18418,30 +19500,35 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabelle9" displayName="Tabelle9" ref="B4:H11" totalsRowShown="0">
-  <autoFilter ref="B4:H11"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Posten">
-      <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabelle467812" displayName="Tabelle467812" ref="B96:I103" totalsRowShown="0">
+  <autoFilter ref="B96:I103"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Posten" dataDxfId="15">
+      <calculatedColumnFormula>B82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="10">
-      <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
+    <tableColumn id="2" name="1" dataDxfId="14">
+      <calculatedColumnFormula>IF(C69=$L$70,$L$70,($E$92-C30)/C69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="9">
-      <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
+    <tableColumn id="3" name="2" dataDxfId="21">
+      <calculatedColumnFormula>IF(D69=$L$70,$L$70,($E$92-D30)/D69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
-      <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
+    <tableColumn id="4" name="3" dataDxfId="20">
+      <calculatedColumnFormula>IF(E69=$L$70,$L$70,($E$92-E30)/E69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="7"/>
-    <tableColumn id="6" name="Status" dataDxfId="6">
-      <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
+    <tableColumn id="5" name="4" dataDxfId="19">
+      <calculatedColumnFormula>IF(F69=$L$70,$L$70,($E$92-F30)/F69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Trend" dataDxfId="5">
-      <calculatedColumnFormula>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
+    <tableColumn id="6" name="5" dataDxfId="18">
+      <calculatedColumnFormula>IF(G69=$L$70,$L$70,($E$92-G30)/G69)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="6" dataDxfId="17">
+      <calculatedColumnFormula>IF(H69=$L$70,$L$70,($E$92-H30)/H69)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="7" dataDxfId="16">
+      <calculatedColumnFormula>IF(I69=$L$70,$L$70,($E$92-I30)/I69)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="SpBC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -18827,24 +19914,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T88"/>
+  <dimension ref="A1:T116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L71" sqref="L71"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.4609375" customWidth="1"/>
-    <col min="2" max="2" width="21.84375" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22.3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -18876,7 +19963,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="str">
         <f>'Budgetierte Kosten'!A2</f>
         <v>Anforderungsanalyse</v>
@@ -18910,7 +19997,7 @@
         <v>144000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" t="str">
         <f>'Budgetierte Kosten'!A3</f>
         <v>Design und Architektur</v>
@@ -18944,7 +20031,7 @@
         <v>172000</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" t="str">
         <f>'Budgetierte Kosten'!A4</f>
         <v>Implementierung</v>
@@ -18978,7 +20065,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" t="str">
         <f>'Budgetierte Kosten'!A5</f>
         <v>Integration und Test</v>
@@ -19012,7 +20099,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" t="str">
         <f>'Budgetierte Kosten'!A6</f>
         <v>Projektmanagement</v>
@@ -19046,7 +20133,7 @@
         <v>154000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" t="str">
         <f>'Budgetierte Kosten'!A7</f>
         <v>Puffer für unerwartetes</v>
@@ -19080,7 +20167,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -19119,12 +20206,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="22.3" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -19150,7 +20237,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" t="str">
         <f t="shared" ref="B17:B23" si="0">B4</f>
         <v>Anforderungsanalyse</v>
@@ -19190,7 +20277,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>Design und Architektur</v>
@@ -19224,7 +20311,7 @@
         <v>87550</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>Implementierung</v>
@@ -19258,7 +20345,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>Integration und Test</v>
@@ -19292,7 +20379,7 @@
         <v>29750</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>Projektmanagement</v>
@@ -19326,7 +20413,7 @@
         <v>204000</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>Puffer für unerwartetes</v>
@@ -19360,7 +20447,7 @@
         <v>353600</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>Materialkosten</v>
@@ -19394,12 +20481,12 @@
         <v>16200</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="22.3" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A27" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -19425,9 +20512,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B30" t="str">
-        <f t="shared" ref="B30:B36" si="1">B4</f>
+        <f t="shared" ref="B30:B36" si="1">B17</f>
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C30" s="28">
@@ -19465,7 +20552,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B31" t="str">
         <f t="shared" si="1"/>
         <v>Design und Architektur</v>
@@ -19499,7 +20586,7 @@
         <v>68800</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B32" t="str">
         <f t="shared" si="1"/>
         <v>Implementierung</v>
@@ -19533,7 +20620,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B33" t="str">
         <f t="shared" si="1"/>
         <v>Integration und Test</v>
@@ -19567,7 +20654,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B34" t="str">
         <f t="shared" si="1"/>
         <v>Projektmanagement</v>
@@ -19601,7 +20688,7 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B35" t="str">
         <f t="shared" si="1"/>
         <v>Puffer für unerwartetes</v>
@@ -19635,7 +20722,7 @@
         <v>30800.000000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B36" t="str">
         <f t="shared" si="1"/>
         <v>Materialkosten</v>
@@ -19669,12 +20756,12 @@
         <v>2940.0000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="22.3" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A40" s="27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>16</v>
       </c>
@@ -19700,7 +20787,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B43" t="str">
         <f>B30</f>
         <v>Anforderungsanalyse</v>
@@ -19740,7 +20827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B44" t="str">
         <f t="shared" ref="B44:B48" si="3">B31</f>
         <v>Design und Architektur</v>
@@ -19774,7 +20861,7 @@
         <v>-18750</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B45" t="str">
         <f t="shared" si="3"/>
         <v>Implementierung</v>
@@ -19808,7 +20895,7 @@
         <v>-2500</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B46" t="str">
         <f t="shared" si="3"/>
         <v>Integration und Test</v>
@@ -19842,7 +20929,7 @@
         <v>-25750</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B47" t="str">
         <f t="shared" si="3"/>
         <v>Projektmanagement</v>
@@ -19876,7 +20963,7 @@
         <v>-127000</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B48" t="str">
         <f t="shared" si="3"/>
         <v>Puffer für unerwartetes</v>
@@ -19910,7 +20997,7 @@
         <v>-322800</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B49" t="str">
         <f>B36</f>
         <v>Materialkosten</v>
@@ -19944,12 +21031,12 @@
         <v>-13260</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="22.3" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A53" s="27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>16</v>
       </c>
@@ -19975,7 +21062,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B56" t="str">
         <f>B43</f>
         <v>Anforderungsanalyse</v>
@@ -20015,7 +21102,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B57" t="str">
         <f t="shared" ref="B57:B61" si="11">B44</f>
         <v>Design und Architektur</v>
@@ -20049,7 +21136,7 @@
         <v>-103200</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B58" t="str">
         <f t="shared" si="11"/>
         <v>Implementierung</v>
@@ -20083,7 +21170,7 @@
         <v>-120000</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B59" t="str">
         <f t="shared" si="11"/>
         <v>Integration und Test</v>
@@ -20117,7 +21204,7 @@
         <v>-12000</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B60" t="str">
         <f t="shared" si="11"/>
         <v>Projektmanagement</v>
@@ -20151,7 +21238,7 @@
         <v>-77000</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B61" t="str">
         <f t="shared" si="11"/>
         <v>Puffer für unerwartetes</v>
@@ -20185,7 +21272,7 @@
         <v>-25199.999999999996</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B62" t="str">
         <f>B49</f>
         <v>Materialkosten</v>
@@ -20219,15 +21306,15 @@
         <v>-18060</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="22.3" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A66" s="27" t="s">
         <v>35</v>
       </c>
       <c r="N66" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>16</v>
       </c>
@@ -20274,7 +21361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B69" t="str">
         <f>B56</f>
         <v>Anforderungsanalyse</v>
@@ -20311,7 +21398,7 @@
         <v>18</v>
       </c>
       <c r="L69" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="M69" t="s">
         <v>37</v>
@@ -20338,7 +21425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B70" t="str">
         <f t="shared" ref="B70:B74" si="25">B57</f>
         <v>Design und Architektur</v>
@@ -20372,13 +21459,13 @@
         <v>0.78583666476299252</v>
       </c>
       <c r="K70" t="s">
+        <v>65</v>
+      </c>
+      <c r="L70" t="s">
         <v>66</v>
       </c>
-      <c r="L70" t="s">
-        <v>67</v>
-      </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B71" t="str">
         <f t="shared" si="25"/>
         <v>Implementierung</v>
@@ -20412,7 +21499,7 @@
         <v>0.94117647058823528</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B72" t="str">
         <f t="shared" si="25"/>
         <v>Integration und Test</v>
@@ -20446,7 +21533,7 @@
         <v>0.13445378151260504</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B73" t="str">
         <f t="shared" si="25"/>
         <v>Projektmanagement</v>
@@ -20480,7 +21567,7 @@
         <v>0.37745098039215685</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B74" t="str">
         <f t="shared" si="25"/>
         <v>Puffer für unerwartetes</v>
@@ -20514,7 +21601,7 @@
         <v>8.7104072398190055E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B75" t="str">
         <f>B62</f>
         <v>Materialkosten</v>
@@ -20548,12 +21635,12 @@
         <v>0.18148148148148152</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="22.3" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A79" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>16</v>
       </c>
@@ -20579,7 +21666,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B82" t="str">
         <f>B69</f>
         <v>Anforderungsanalyse</v>
@@ -20622,7 +21709,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B83" t="str">
         <f t="shared" ref="B83:B87" si="38">B70</f>
         <v>Design und Architektur</v>
@@ -20656,7 +21743,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B84" t="str">
         <f t="shared" si="38"/>
         <v>Implementierung</v>
@@ -20690,7 +21777,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B85" t="str">
         <f t="shared" si="38"/>
         <v>Integration und Test</v>
@@ -20724,7 +21811,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B86" t="str">
         <f t="shared" si="38"/>
         <v>Projektmanagement</v>
@@ -20758,7 +21845,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B87" t="str">
         <f t="shared" si="38"/>
         <v>Puffer für unerwartetes</v>
@@ -20792,7 +21879,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B88" t="str">
         <f>B75</f>
         <v>Materialkosten</v>
@@ -20824,12 +21911,574 @@
       <c r="I88" s="29">
         <f t="shared" ref="I88" si="44">IF(I10=0,"-",I36/I10)</f>
         <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A92" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E92">
+        <f>1.25 * 10^6</f>
+        <v>1250000</v>
+      </c>
+      <c r="F92" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A94" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" t="s">
+        <v>21</v>
+      </c>
+      <c r="F96" t="s">
+        <v>22</v>
+      </c>
+      <c r="G96" t="s">
+        <v>23</v>
+      </c>
+      <c r="H96" t="s">
+        <v>24</v>
+      </c>
+      <c r="I96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B97" t="str">
+        <f t="shared" ref="B97:B103" si="45">B82</f>
+        <v>Anforderungsanalyse</v>
+      </c>
+      <c r="C97" s="29">
+        <f t="shared" ref="C97:I103" si="46">IF(C69=$L$70,$L$70,($E$92-C30)/C69)</f>
+        <v>3119702.3809523811</v>
+      </c>
+      <c r="D97" s="29">
+        <f t="shared" si="46"/>
+        <v>22050416.666666664</v>
+      </c>
+      <c r="E97" s="29">
+        <f t="shared" si="46"/>
+        <v>11231947.222222222</v>
+      </c>
+      <c r="F97" s="29">
+        <f t="shared" si="46"/>
+        <v>3775440.2777777775</v>
+      </c>
+      <c r="G97" s="29">
+        <f t="shared" si="46"/>
+        <v>2211204.1666666665</v>
+      </c>
+      <c r="H97" s="29">
+        <f t="shared" si="46"/>
+        <v>1331321.3541666667</v>
+      </c>
+      <c r="I97" s="29">
+        <f t="shared" si="46"/>
+        <v>1168380.0925925926</v>
+      </c>
+      <c r="K97" t="s">
+        <v>18</v>
+      </c>
+      <c r="L97" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B98" t="str">
+        <f t="shared" si="45"/>
+        <v>Design und Architektur</v>
+      </c>
+      <c r="C98" s="29" t="str">
+        <f t="shared" ref="C98:I98" si="47">IF(C70=$L$70,$L$70,($E$92-C31)/C70)</f>
+        <v>-</v>
+      </c>
+      <c r="D98" s="29" t="str">
+        <f t="shared" si="47"/>
+        <v>-</v>
+      </c>
+      <c r="E98" s="29" t="str">
+        <f t="shared" si="47"/>
+        <v>-</v>
+      </c>
+      <c r="F98" s="29">
+        <f t="shared" si="47"/>
+        <v>20390192.307692308</v>
+      </c>
+      <c r="G98" s="29">
+        <f t="shared" si="47"/>
+        <v>15435291.666666666</v>
+      </c>
+      <c r="H98" s="29">
+        <f t="shared" si="47"/>
+        <v>6421772.3684210526</v>
+      </c>
+      <c r="I98" s="29">
+        <f t="shared" si="47"/>
+        <v>1503111.3372093025</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B99" t="str">
+        <f t="shared" si="45"/>
+        <v>Implementierung</v>
+      </c>
+      <c r="C99" s="29" t="str">
+        <f t="shared" ref="C99:I99" si="48">IF(C71=$L$70,$L$70,($E$92-C32)/C71)</f>
+        <v>-</v>
+      </c>
+      <c r="D99" s="29" t="str">
+        <f t="shared" si="48"/>
+        <v>-</v>
+      </c>
+      <c r="E99" s="29" t="str">
+        <f t="shared" si="48"/>
+        <v>-</v>
+      </c>
+      <c r="F99" s="29" t="str">
+        <f t="shared" si="48"/>
+        <v>-</v>
+      </c>
+      <c r="G99" s="29" t="str">
+        <f t="shared" si="48"/>
+        <v>-</v>
+      </c>
+      <c r="H99" s="29">
+        <f t="shared" si="48"/>
+        <v>2350401.7857142854</v>
+      </c>
+      <c r="I99" s="29">
+        <f t="shared" si="48"/>
+        <v>1285625</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B100" t="str">
+        <f t="shared" si="45"/>
+        <v>Integration und Test</v>
+      </c>
+      <c r="C100" s="29" t="str">
+        <f t="shared" ref="C100:I100" si="49">IF(C72=$L$70,$L$70,($E$92-C33)/C72)</f>
+        <v>-</v>
+      </c>
+      <c r="D100" s="29" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
+      </c>
+      <c r="E100" s="29" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
+      </c>
+      <c r="F100" s="29" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
+      </c>
+      <c r="G100" s="29" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
+      </c>
+      <c r="H100" s="29" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
+      </c>
+      <c r="I100" s="29">
+        <f t="shared" si="49"/>
+        <v>9267125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B101" t="str">
+        <f t="shared" si="45"/>
+        <v>Projektmanagement</v>
+      </c>
+      <c r="C101" s="29">
+        <f t="shared" ref="C101:I101" si="50">IF(C73=$L$70,$L$70,($E$92-C34)/C73)</f>
+        <v>18085295.454545457</v>
+      </c>
+      <c r="D101" s="29">
+        <f t="shared" si="50"/>
+        <v>53031500</v>
+      </c>
+      <c r="E101" s="29">
+        <f t="shared" si="50"/>
+        <v>15970984.848484848</v>
+      </c>
+      <c r="F101" s="29">
+        <f t="shared" si="50"/>
+        <v>10713477.272727273</v>
+      </c>
+      <c r="G101" s="29">
+        <f t="shared" si="50"/>
+        <v>6269393.9393939395</v>
+      </c>
+      <c r="H101" s="29">
+        <f t="shared" si="50"/>
+        <v>4240083.333333333</v>
+      </c>
+      <c r="I101" s="29">
+        <f t="shared" si="50"/>
+        <v>3107688.3116883119</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B102" t="str">
+        <f t="shared" si="45"/>
+        <v>Puffer für unerwartetes</v>
+      </c>
+      <c r="C102" s="29">
+        <f t="shared" ref="C102:I102" si="51">IF(C74=$L$70,$L$70,($E$92-C35)/C74)</f>
+        <v>26548900</v>
+      </c>
+      <c r="D102" s="29">
+        <f t="shared" si="51"/>
+        <v>260145900.00000003</v>
+      </c>
+      <c r="E102" s="29">
+        <f t="shared" si="51"/>
+        <v>157301566.66666666</v>
+      </c>
+      <c r="F102" s="29">
+        <f t="shared" si="51"/>
+        <v>66231415.625000007</v>
+      </c>
+      <c r="G102" s="29">
+        <f t="shared" si="51"/>
+        <v>35602816.666666672</v>
+      </c>
+      <c r="H102" s="29">
+        <f t="shared" si="51"/>
+        <v>19867663.888888888</v>
+      </c>
+      <c r="I102" s="29">
+        <f t="shared" si="51"/>
+        <v>13997049.350649349</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B103" t="str">
+        <f t="shared" si="45"/>
+        <v>Materialkosten</v>
+      </c>
+      <c r="C103" s="29">
+        <f t="shared" ref="C103:I103" si="52">IF(C75=$L$70,$L$70,($E$92-C36)/C75)</f>
+        <v>62498000</v>
+      </c>
+      <c r="D103" s="29">
+        <f t="shared" si="52"/>
+        <v>27340250</v>
+      </c>
+      <c r="E103" s="29">
+        <f t="shared" si="52"/>
+        <v>14578433.333333334</v>
+      </c>
+      <c r="F103" s="29">
+        <f t="shared" si="52"/>
+        <v>9993600</v>
+      </c>
+      <c r="G103" s="29">
+        <f t="shared" si="52"/>
+        <v>7107984.615384615</v>
+      </c>
+      <c r="H103" s="29">
+        <f t="shared" si="52"/>
+        <v>9750625</v>
+      </c>
+      <c r="I103" s="29">
+        <f t="shared" si="52"/>
+        <v>6871555.1020408152</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A107" s="33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>16</v>
+      </c>
+      <c r="C109" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" t="s">
+        <v>20</v>
+      </c>
+      <c r="E109" t="s">
+        <v>21</v>
+      </c>
+      <c r="F109" t="s">
+        <v>22</v>
+      </c>
+      <c r="G109" t="s">
+        <v>23</v>
+      </c>
+      <c r="H109" t="s">
+        <v>24</v>
+      </c>
+      <c r="I109" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B110" t="str">
+        <f t="shared" ref="B110:B116" si="53">B97</f>
+        <v>Anforderungsanalyse</v>
+      </c>
+      <c r="C110" s="29">
+        <f t="shared" ref="C110:I116" si="54">IF(C69=$L$70,$L$70,$E$92/C69)</f>
+        <v>3162202.3809523811</v>
+      </c>
+      <c r="D110" s="29">
+        <f t="shared" si="54"/>
+        <v>22135416.666666664</v>
+      </c>
+      <c r="E110" s="29">
+        <f t="shared" si="54"/>
+        <v>11362847.222222222</v>
+      </c>
+      <c r="F110" s="29">
+        <f t="shared" si="54"/>
+        <v>3910590.2777777775</v>
+      </c>
+      <c r="G110" s="29">
+        <f t="shared" si="54"/>
+        <v>2346354.1666666665</v>
+      </c>
+      <c r="H110" s="29">
+        <f t="shared" si="54"/>
+        <v>1466471.3541666667</v>
+      </c>
+      <c r="I110" s="29">
+        <f t="shared" si="54"/>
+        <v>1303530.0925925926</v>
+      </c>
+      <c r="K110" t="s">
+        <v>18</v>
+      </c>
+      <c r="L110" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B111" t="str">
+        <f t="shared" si="53"/>
+        <v>Design und Architektur</v>
+      </c>
+      <c r="C111" s="29" t="str">
+        <f t="shared" ref="C111:I111" si="55">IF(C70=$L$70,$L$70,$E$92/C70)</f>
+        <v>-</v>
+      </c>
+      <c r="D111" s="29" t="str">
+        <f t="shared" si="55"/>
+        <v>-</v>
+      </c>
+      <c r="E111" s="29" t="str">
+        <f t="shared" si="55"/>
+        <v>-</v>
+      </c>
+      <c r="F111" s="29">
+        <f t="shared" si="55"/>
+        <v>20432692.307692308</v>
+      </c>
+      <c r="G111" s="29">
+        <f t="shared" si="55"/>
+        <v>15494791.666666666</v>
+      </c>
+      <c r="H111" s="29">
+        <f t="shared" si="55"/>
+        <v>6500822.3684210526</v>
+      </c>
+      <c r="I111" s="29">
+        <f t="shared" si="55"/>
+        <v>1590661.3372093025</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B112" t="str">
+        <f t="shared" si="53"/>
+        <v>Implementierung</v>
+      </c>
+      <c r="C112" s="29" t="str">
+        <f t="shared" ref="C112:I112" si="56">IF(C71=$L$70,$L$70,$E$92/C71)</f>
+        <v>-</v>
+      </c>
+      <c r="D112" s="29" t="str">
+        <f t="shared" si="56"/>
+        <v>-</v>
+      </c>
+      <c r="E112" s="29" t="str">
+        <f t="shared" si="56"/>
+        <v>-</v>
+      </c>
+      <c r="F112" s="29" t="str">
+        <f t="shared" si="56"/>
+        <v>-</v>
+      </c>
+      <c r="G112" s="29" t="str">
+        <f t="shared" si="56"/>
+        <v>-</v>
+      </c>
+      <c r="H112" s="29">
+        <f t="shared" si="56"/>
+        <v>2371651.7857142854</v>
+      </c>
+      <c r="I112" s="29">
+        <f t="shared" si="56"/>
+        <v>1328125</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B113" t="str">
+        <f t="shared" si="53"/>
+        <v>Integration und Test</v>
+      </c>
+      <c r="C113" s="29" t="str">
+        <f t="shared" ref="C113:I113" si="57">IF(C72=$L$70,$L$70,$E$92/C72)</f>
+        <v>-</v>
+      </c>
+      <c r="D113" s="29" t="str">
+        <f t="shared" si="57"/>
+        <v>-</v>
+      </c>
+      <c r="E113" s="29" t="str">
+        <f t="shared" si="57"/>
+        <v>-</v>
+      </c>
+      <c r="F113" s="29" t="str">
+        <f t="shared" si="57"/>
+        <v>-</v>
+      </c>
+      <c r="G113" s="29" t="str">
+        <f t="shared" si="57"/>
+        <v>-</v>
+      </c>
+      <c r="H113" s="29" t="str">
+        <f t="shared" si="57"/>
+        <v>-</v>
+      </c>
+      <c r="I113" s="29">
+        <f t="shared" si="57"/>
+        <v>9296875</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B114" t="str">
+        <f t="shared" si="53"/>
+        <v>Projektmanagement</v>
+      </c>
+      <c r="C114" s="29">
+        <f t="shared" ref="C114:I114" si="58">IF(C73=$L$70,$L$70,$E$92/C73)</f>
+        <v>18110795.454545457</v>
+      </c>
+      <c r="D114" s="29">
+        <f t="shared" si="58"/>
+        <v>53125000</v>
+      </c>
+      <c r="E114" s="29">
+        <f t="shared" si="58"/>
+        <v>16098484.848484848</v>
+      </c>
+      <c r="F114" s="29">
+        <f t="shared" si="58"/>
+        <v>10866477.272727273</v>
+      </c>
+      <c r="G114" s="29">
+        <f t="shared" si="58"/>
+        <v>6439393.9393939395</v>
+      </c>
+      <c r="H114" s="29">
+        <f t="shared" si="58"/>
+        <v>4427083.333333333</v>
+      </c>
+      <c r="I114" s="29">
+        <f t="shared" si="58"/>
+        <v>3311688.3116883119</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B115" t="str">
+        <f t="shared" si="53"/>
+        <v>Puffer für unerwartetes</v>
+      </c>
+      <c r="C115" s="29">
+        <f t="shared" ref="C115:I115" si="59">IF(C74=$L$70,$L$70,$E$92/C74)</f>
+        <v>26562500</v>
+      </c>
+      <c r="D115" s="29">
+        <f t="shared" si="59"/>
+        <v>260312500.00000003</v>
+      </c>
+      <c r="E115" s="29">
+        <f t="shared" si="59"/>
+        <v>157604166.66666666</v>
+      </c>
+      <c r="F115" s="29">
+        <f t="shared" si="59"/>
+        <v>66572265.625000007</v>
+      </c>
+      <c r="G115" s="29">
+        <f t="shared" si="59"/>
+        <v>35947916.666666672</v>
+      </c>
+      <c r="H115" s="29">
+        <f t="shared" si="59"/>
+        <v>20217013.888888888</v>
+      </c>
+      <c r="I115" s="29">
+        <f t="shared" si="59"/>
+        <v>14350649.350649349</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B116" t="str">
+        <f t="shared" si="53"/>
+        <v>Materialkosten</v>
+      </c>
+      <c r="C116" s="29">
+        <f t="shared" ref="C116:I116" si="60">IF(C75=$L$70,$L$70,$E$92/C75)</f>
+        <v>62500000</v>
+      </c>
+      <c r="D116" s="29">
+        <f t="shared" si="60"/>
+        <v>27343750</v>
+      </c>
+      <c r="E116" s="29">
+        <f t="shared" si="60"/>
+        <v>14583333.333333334</v>
+      </c>
+      <c r="F116" s="29">
+        <f t="shared" si="60"/>
+        <v>10000000</v>
+      </c>
+      <c r="G116" s="29">
+        <f t="shared" si="60"/>
+        <v>7115384.615384615</v>
+      </c>
+      <c r="H116" s="29">
+        <f t="shared" si="60"/>
+        <v>9765625</v>
+      </c>
+      <c r="I116" s="29">
+        <f t="shared" si="60"/>
+        <v>6887755.1020408152</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <tableParts count="8">
+  <tableParts count="10">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -20838,6 +22487,8 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
@@ -20846,62 +22497,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.23046875" customWidth="1"/>
-    <col min="5" max="5" width="16.07421875" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.4609375" customWidth="1"/>
-    <col min="10" max="10" width="18.3828125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="22.3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>45</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>47</v>
       </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="str">
         <f>Kennzahlen!B56</f>
         <v>Anforderungsanalyse</v>
@@ -20931,7 +22582,7 @@
         <v>POS</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" t="str">
         <f>Kennzahlen!B57</f>
         <v>Design und Architektur</v>
@@ -20961,13 +22612,13 @@
         <v>POS</v>
       </c>
       <c r="J6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" t="s">
         <v>52</v>
       </c>
-      <c r="K6" t="s">
-        <v>53</v>
-      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="str">
         <f>Kennzahlen!B58</f>
         <v>Implementierung</v>
@@ -20997,13 +22648,13 @@
         <v>POS</v>
       </c>
       <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" t="s">
         <v>54</v>
       </c>
-      <c r="K7" t="s">
-        <v>55</v>
-      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="str">
         <f>Kennzahlen!B59</f>
         <v>Integration und Test</v>
@@ -21033,13 +22684,13 @@
         <v>-</v>
       </c>
       <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
         <v>56</v>
       </c>
-      <c r="K8" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" t="str">
         <f>Kennzahlen!B60</f>
         <v>Projektmanagement</v>
@@ -21069,7 +22720,7 @@
         <v>POS</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" t="str">
         <f>Kennzahlen!B61</f>
         <v>Puffer für unerwartetes</v>
@@ -21099,13 +22750,13 @@
         <v>EQ</v>
       </c>
       <c r="J10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" t="str">
         <f>Kennzahlen!B62</f>
         <v>Materialkosten</v>
@@ -21135,57 +22786,57 @@
         <v>POS</v>
       </c>
       <c r="J11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J12" t="s">
-        <v>65</v>
-      </c>
-      <c r="K12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K13">
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="22.3" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
         <v>46</v>
       </c>
-      <c r="F17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>47</v>
       </c>
-      <c r="H17" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" t="str">
         <f>Kennzahlen!B69</f>
         <v>Anforderungsanalyse</v>
@@ -21211,7 +22862,7 @@
         <v>Gelb</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" t="str">
         <f>Kennzahlen!B70</f>
         <v>Design und Architektur</v>
@@ -21237,7 +22888,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" t="str">
         <f>Kennzahlen!B71</f>
         <v>Implementierung</v>
@@ -21263,7 +22914,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" t="str">
         <f>Kennzahlen!B72</f>
         <v>Integration und Test</v>
@@ -21289,7 +22940,7 @@
         <v>Grün</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" t="str">
         <f>Kennzahlen!B73</f>
         <v>Projektmanagement</v>
@@ -21315,7 +22966,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" t="str">
         <f>Kennzahlen!B74</f>
         <v>Puffer für unerwartetes</v>
@@ -21341,7 +22992,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" t="str">
         <f>Kennzahlen!B75</f>
         <v>Materialkosten</v>
@@ -21369,13 +23020,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D11 C18:D24">
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThanOrEqual">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="lessThan">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="lessThan">
       <formula>$K$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21434,11 +23085,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A66" zoomScale="51" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -21450,23 +23101,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.3828125" customWidth="1"/>
-    <col min="2" max="2" width="11.15234375" customWidth="1"/>
-    <col min="3" max="3" width="10.15234375" customWidth="1"/>
-    <col min="4" max="4" width="10.3046875" customWidth="1"/>
-    <col min="5" max="13" width="9.3828125" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="13" width="9.42578125" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="15.3828125" customWidth="1"/>
-    <col min="16" max="16" width="14.84375" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -21513,7 +23164,7 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -21565,7 +23216,7 @@
         <v>144000</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -21617,7 +23268,7 @@
         <v>236000</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -21669,7 +23320,7 @@
         <v>392000</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -21721,7 +23372,7 @@
         <v>252000</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -21773,7 +23424,7 @@
         <v>286000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -21825,7 +23476,7 @@
         <v>104000</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -21890,11 +23541,11 @@
         <v>1414000</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
@@ -21955,7 +23606,7 @@
       </c>
       <c r="P10" s="10"/>
     </row>
-    <row r="11" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
@@ -22007,7 +23658,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="2" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -22065,7 +23716,7 @@
       </c>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -22080,7 +23731,7 @@
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
     </row>
-    <row r="14" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
@@ -22119,19 +23770,19 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.3828125" customWidth="1"/>
-    <col min="2" max="8" width="9.3828125" customWidth="1"/>
-    <col min="9" max="9" width="13.69140625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="12.3046875" style="20" customWidth="1"/>
-    <col min="11" max="12" width="11.3828125" style="20" customWidth="1"/>
-    <col min="13" max="13" width="12.3046875" style="20" customWidth="1"/>
-    <col min="14" max="15" width="11.3828125" style="20" customWidth="1"/>
-    <col min="16" max="16" width="12.3046875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="20" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="20" customWidth="1"/>
+    <col min="11" max="12" width="11.42578125" style="20" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="20" customWidth="1"/>
+    <col min="14" max="15" width="11.42578125" style="20" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -22163,7 +23814,7 @@
       <c r="O1" s="22"/>
       <c r="P1" s="23"/>
     </row>
-    <row r="2" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -22189,7 +23840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -22215,7 +23866,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
@@ -22241,7 +23892,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
@@ -22267,7 +23918,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
@@ -22293,7 +23944,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
@@ -22319,7 +23970,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
         <f>'Budgetierte Kosten'!A8</f>
         <v>Summe Personenstunden pro Monat</v>
@@ -22353,7 +24004,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -22363,7 +24014,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -22396,7 +24047,7 @@
         <v>80750</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -22430,7 +24081,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -22471,7 +24122,7 @@
       <c r="O12" s="24"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="15" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -22495,16 +24146,16 @@
       <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.3828125" customWidth="1"/>
-    <col min="2" max="3" width="10.15234375" customWidth="1"/>
-    <col min="4" max="8" width="11.3828125" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="11" width="4" customWidth="1"/>
     <col min="12" max="13" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -22535,7 +24186,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="str">
         <f>'Budgetierte Kosten'!A2</f>
         <v>Anforderungsanalyse</v>
@@ -22562,7 +24213,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="str">
         <f>'Budgetierte Kosten'!A3</f>
         <v>Design und Architektur</v>
@@ -22589,7 +24240,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="str">
         <f>'Budgetierte Kosten'!A4</f>
         <v>Implementierung</v>
@@ -22616,7 +24267,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="str">
         <f>'Budgetierte Kosten'!A5</f>
         <v>Integration und Test</v>
@@ -22643,7 +24294,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="str">
         <f>'Budgetierte Kosten'!A6</f>
         <v>Projektmanagement</v>
@@ -22670,7 +24321,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="str">
         <f>'Budgetierte Kosten'!A7</f>
         <v>Puffer für unerwartetes</v>
@@ -22697,7 +24348,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -22728,7 +24379,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
changed BAC to end PV
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
@@ -546,10 +546,14 @@
   </cellStyles>
   <dxfs count="73">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -558,10 +562,17 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -615,6 +626,24 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -636,45 +665,10 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -746,7 +740,13 @@
       <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
@@ -4869,25 +4869,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3119702.3809523811</c:v>
+                  <c:v>3752142.8571428573</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22050416.666666664</c:v>
+                  <c:v>26477500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11231947.222222222</c:v>
+                  <c:v>13504516.666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3775440.2777777775</c:v>
+                  <c:v>4557558.333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2211204.1666666665</c:v>
+                  <c:v>2680475</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1331321.3541666667</c:v>
+                  <c:v>1624615.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1168380.0925925926</c:v>
+                  <c:v>1429086.1111111112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19185,28 +19185,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabelle46781213" displayName="Tabelle46781213" ref="B109:I116" totalsRowShown="0">
   <autoFilter ref="B109:I116"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Posten" dataDxfId="1">
+    <tableColumn id="1" name="Posten" dataDxfId="24">
       <calculatedColumnFormula>B97</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="0">
+    <tableColumn id="2" name="1" dataDxfId="23">
       <calculatedColumnFormula>IF(C69=$L$70,$L$70,$E$92/C69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="7">
+    <tableColumn id="3" name="2" dataDxfId="22">
       <calculatedColumnFormula>IF(D69=$L$70,$L$70,$E$92/D69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" dataDxfId="6">
+    <tableColumn id="4" name="3" dataDxfId="21">
       <calculatedColumnFormula>IF(E69=$L$70,$L$70,$E$92/E69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" dataDxfId="5">
+    <tableColumn id="5" name="4" dataDxfId="20">
       <calculatedColumnFormula>IF(F69=$L$70,$L$70,$E$92/F69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" dataDxfId="4">
+    <tableColumn id="6" name="5" dataDxfId="19">
       <calculatedColumnFormula>IF(G69=$L$70,$L$70,$E$92/G69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" dataDxfId="3">
+    <tableColumn id="7" name="6" dataDxfId="18">
       <calculatedColumnFormula>IF(H69=$L$70,$L$70,$E$92/H69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="2">
+    <tableColumn id="8" name="7" dataDxfId="17">
       <calculatedColumnFormula>IF(I69=$L$70,$L$70,$E$92/I69)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -19221,20 +19221,20 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="34">
+    <tableColumn id="2" name="CPI" dataDxfId="10">
       <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="33">
+    <tableColumn id="3" name="SPI" dataDxfId="9">
       <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="32">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="31"/>
-    <tableColumn id="6" name="Status" dataDxfId="30">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="7"/>
+    <tableColumn id="6" name="Status" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Trend" dataDxfId="29">
+    <tableColumn id="7" name="Trend" dataDxfId="5">
       <calculatedColumnFormula>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -19249,19 +19249,19 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="28">
+    <tableColumn id="2" name="CPI" dataDxfId="4">
       <calculatedColumnFormula>Kennzahlen!H69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="27">
+    <tableColumn id="3" name="SPI" dataDxfId="3">
       <calculatedColumnFormula>Kennzahlen!H82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="26">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="2">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="25">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="1">
       <calculatedColumnFormula>Kennzahlen!H4/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Status" dataDxfId="24">
+    <tableColumn id="6" name="Status" dataDxfId="0">
       <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Trend"/>
@@ -19283,10 +19283,10 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" name="Posten" dataDxfId="22">
+    <tableColumn id="1" name="Posten" dataDxfId="58">
       <calculatedColumnFormula>B17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="58">
+    <tableColumn id="2" name="1" dataDxfId="57">
       <calculatedColumnFormula>C4*'Fertigstellungsgrad der Akt.'!B2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -19325,18 +19325,18 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" name="Posten" dataDxfId="23">
+    <tableColumn id="1" name="Posten" dataDxfId="56">
       <calculatedColumnFormula>B4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="57">
+    <tableColumn id="2" name="1" dataDxfId="55">
       <calculatedColumnFormula>'Tatsächliche Kosten'!B2*'Tatsächliche Kosten'!$B$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="56"/>
-    <tableColumn id="4" name="3" dataDxfId="55"/>
-    <tableColumn id="5" name="4" dataDxfId="54"/>
-    <tableColumn id="6" name="5" dataDxfId="53"/>
-    <tableColumn id="7" name="6" dataDxfId="52"/>
-    <tableColumn id="8" name="7" dataDxfId="51"/>
+    <tableColumn id="3" name="2" dataDxfId="54"/>
+    <tableColumn id="4" name="3" dataDxfId="53"/>
+    <tableColumn id="5" name="4" dataDxfId="52"/>
+    <tableColumn id="6" name="5" dataDxfId="51"/>
+    <tableColumn id="7" name="6" dataDxfId="50"/>
+    <tableColumn id="8" name="7" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -19358,7 +19358,7 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="50">
+    <tableColumn id="2" name="1" dataDxfId="48">
       <calculatedColumnFormula>C30-C17</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -19391,7 +19391,7 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B43</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="49">
+    <tableColumn id="2" name="1" dataDxfId="47">
       <calculatedColumnFormula>C30-C4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -19424,25 +19424,25 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="48">
+    <tableColumn id="2" name="1" dataDxfId="46">
       <calculatedColumnFormula>IF(C17=0,$L$70,C30/C17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="47">
+    <tableColumn id="3" name="2" dataDxfId="45">
       <calculatedColumnFormula>IF(D17=0,$L$70,D30/D17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" dataDxfId="46">
+    <tableColumn id="4" name="3" dataDxfId="44">
       <calculatedColumnFormula>IF(E17=0,$L$70,E30/E17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" dataDxfId="45">
+    <tableColumn id="5" name="4" dataDxfId="43">
       <calculatedColumnFormula>IF(F17=0,$L$70,F30/F17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" dataDxfId="44">
+    <tableColumn id="6" name="5" dataDxfId="42">
       <calculatedColumnFormula>IF(G17=0,$L$70,G30/G17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" dataDxfId="43">
+    <tableColumn id="7" name="6" dataDxfId="41">
       <calculatedColumnFormula>IF(H17=0,$L$70,H30/H17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="42">
+    <tableColumn id="8" name="7" dataDxfId="40">
       <calculatedColumnFormula>IF(I17=0,"-",I30/I17)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -19457,25 +19457,25 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="41">
+    <tableColumn id="2" name="1" dataDxfId="39">
       <calculatedColumnFormula>IF(C4=0,$L$70,C30/C4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="40">
+    <tableColumn id="3" name="2" dataDxfId="38">
       <calculatedColumnFormula>IF(D4=0,$L$70,D30/D4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" dataDxfId="39">
+    <tableColumn id="4" name="3" dataDxfId="37">
       <calculatedColumnFormula>IF(E4=0,$L$70,E30/E4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" dataDxfId="38">
+    <tableColumn id="5" name="4" dataDxfId="36">
       <calculatedColumnFormula>IF(F4=0,$L$70,F30/F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" dataDxfId="37">
+    <tableColumn id="6" name="5" dataDxfId="35">
       <calculatedColumnFormula>IF(G4=0,$L$70,G30/G4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" dataDxfId="36">
+    <tableColumn id="7" name="6" dataDxfId="34">
       <calculatedColumnFormula>IF(H4=0,$L$70,H30/H4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="35">
+    <tableColumn id="8" name="7" dataDxfId="33">
       <calculatedColumnFormula>IF(I4=0,"-",I30/I4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -19503,28 +19503,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabelle467812" displayName="Tabelle467812" ref="B96:I103" totalsRowShown="0">
   <autoFilter ref="B96:I103"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Posten" dataDxfId="15">
+    <tableColumn id="1" name="Posten" dataDxfId="32">
       <calculatedColumnFormula>B82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" dataDxfId="14">
+    <tableColumn id="2" name="1" dataDxfId="31">
       <calculatedColumnFormula>IF(C69=$L$70,$L$70,($E$92-C30)/C69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" dataDxfId="21">
+    <tableColumn id="3" name="2" dataDxfId="30">
       <calculatedColumnFormula>IF(D69=$L$70,$L$70,($E$92-D30)/D69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" dataDxfId="20">
+    <tableColumn id="4" name="3" dataDxfId="29">
       <calculatedColumnFormula>IF(E69=$L$70,$L$70,($E$92-E30)/E69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" dataDxfId="19">
+    <tableColumn id="5" name="4" dataDxfId="28">
       <calculatedColumnFormula>IF(F69=$L$70,$L$70,($E$92-F30)/F69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" dataDxfId="18">
+    <tableColumn id="6" name="5" dataDxfId="27">
       <calculatedColumnFormula>IF(G69=$L$70,$L$70,($E$92-G30)/G69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" dataDxfId="17">
+    <tableColumn id="7" name="6" dataDxfId="26">
       <calculatedColumnFormula>IF(H69=$L$70,$L$70,($E$92-H30)/H69)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" dataDxfId="16">
+    <tableColumn id="8" name="7" dataDxfId="25">
       <calculatedColumnFormula>IF(I69=$L$70,$L$70,($E$92-I30)/I69)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -19916,8 +19916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T116"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="J90" sqref="J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21918,8 +21918,8 @@
         <v>71</v>
       </c>
       <c r="E92">
-        <f>1.25 * 10^6</f>
-        <v>1250000</v>
+        <f>'Budgetierte Kosten'!$P$11</f>
+        <v>1500000</v>
       </c>
       <c r="F92" t="s">
         <v>70</v>
@@ -21962,32 +21962,32 @@
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C97" s="29">
-        <f t="shared" ref="C97:I103" si="46">IF(C69=$L$70,$L$70,($E$92-C30)/C69)</f>
-        <v>3119702.3809523811</v>
+        <f t="shared" ref="C97:I97" si="46">IF(C69=$L$70,$L$70,($E$92-C30)/C69)</f>
+        <v>3752142.8571428573</v>
       </c>
       <c r="D97" s="29">
         <f t="shared" si="46"/>
-        <v>22050416.666666664</v>
+        <v>26477500</v>
       </c>
       <c r="E97" s="29">
         <f t="shared" si="46"/>
-        <v>11231947.222222222</v>
+        <v>13504516.666666666</v>
       </c>
       <c r="F97" s="29">
         <f t="shared" si="46"/>
-        <v>3775440.2777777775</v>
+        <v>4557558.333333333</v>
       </c>
       <c r="G97" s="29">
         <f t="shared" si="46"/>
-        <v>2211204.1666666665</v>
+        <v>2680475</v>
       </c>
       <c r="H97" s="29">
         <f t="shared" si="46"/>
-        <v>1331321.3541666667</v>
+        <v>1624615.625</v>
       </c>
       <c r="I97" s="29">
         <f t="shared" si="46"/>
-        <v>1168380.0925925926</v>
+        <v>1429086.1111111112</v>
       </c>
       <c r="K97" t="s">
         <v>18</v>
@@ -22015,19 +22015,19 @@
       </c>
       <c r="F98" s="29">
         <f t="shared" si="47"/>
-        <v>20390192.307692308</v>
+        <v>24476730.769230768</v>
       </c>
       <c r="G98" s="29">
         <f t="shared" si="47"/>
-        <v>15435291.666666666</v>
+        <v>18534250</v>
       </c>
       <c r="H98" s="29">
         <f t="shared" si="47"/>
-        <v>6421772.3684210526</v>
+        <v>7721936.8421052629</v>
       </c>
       <c r="I98" s="29">
         <f t="shared" si="47"/>
-        <v>1503111.3372093025</v>
+        <v>1821243.6046511629</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.2">
@@ -22057,11 +22057,11 @@
       </c>
       <c r="H99" s="29">
         <f t="shared" si="48"/>
-        <v>2350401.7857142854</v>
+        <v>2824732.1428571427</v>
       </c>
       <c r="I99" s="29">
         <f t="shared" si="48"/>
-        <v>1285625</v>
+        <v>1551250</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.2">
@@ -22095,7 +22095,7 @@
       </c>
       <c r="I100" s="29">
         <f t="shared" si="49"/>
-        <v>9267125</v>
+        <v>11126500</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.2">
@@ -22105,31 +22105,31 @@
       </c>
       <c r="C101" s="29">
         <f t="shared" ref="C101:I101" si="50">IF(C73=$L$70,$L$70,($E$92-C34)/C73)</f>
-        <v>18085295.454545457</v>
+        <v>21707454.545454547</v>
       </c>
       <c r="D101" s="29">
         <f t="shared" si="50"/>
-        <v>53031500</v>
+        <v>63656500</v>
       </c>
       <c r="E101" s="29">
         <f t="shared" si="50"/>
-        <v>15970984.848484848</v>
+        <v>19190681.818181816</v>
       </c>
       <c r="F101" s="29">
         <f t="shared" si="50"/>
-        <v>10713477.272727273</v>
+        <v>12886772.727272728</v>
       </c>
       <c r="G101" s="29">
         <f t="shared" si="50"/>
-        <v>6269393.9393939395</v>
+        <v>7557272.7272727275</v>
       </c>
       <c r="H101" s="29">
         <f t="shared" si="50"/>
-        <v>4240083.333333333</v>
+        <v>5125500</v>
       </c>
       <c r="I101" s="29">
         <f t="shared" si="50"/>
-        <v>3107688.3116883119</v>
+        <v>3770025.9740259741</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.2">
@@ -22139,31 +22139,31 @@
       </c>
       <c r="C102" s="29">
         <f t="shared" ref="C102:I102" si="51">IF(C74=$L$70,$L$70,($E$92-C35)/C74)</f>
-        <v>26548900</v>
+        <v>31861400</v>
       </c>
       <c r="D102" s="29">
         <f t="shared" si="51"/>
-        <v>260145900.00000003</v>
+        <v>312208400</v>
       </c>
       <c r="E102" s="29">
         <f t="shared" si="51"/>
-        <v>157301566.66666666</v>
+        <v>188822400</v>
       </c>
       <c r="F102" s="29">
         <f t="shared" si="51"/>
-        <v>66231415.625000007</v>
+        <v>79545868.75</v>
       </c>
       <c r="G102" s="29">
         <f t="shared" si="51"/>
-        <v>35602816.666666672</v>
+        <v>42792400</v>
       </c>
       <c r="H102" s="29">
         <f t="shared" si="51"/>
-        <v>19867663.888888888</v>
+        <v>23911066.666666668</v>
       </c>
       <c r="I102" s="29">
         <f t="shared" si="51"/>
-        <v>13997049.350649349</v>
+        <v>16867179.220779218</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
@@ -22173,31 +22173,31 @@
       </c>
       <c r="C103" s="29">
         <f t="shared" ref="C103:I103" si="52">IF(C75=$L$70,$L$70,($E$92-C36)/C75)</f>
-        <v>62498000</v>
+        <v>74998000</v>
       </c>
       <c r="D103" s="29">
         <f t="shared" si="52"/>
-        <v>27340250</v>
+        <v>32809000</v>
       </c>
       <c r="E103" s="29">
         <f t="shared" si="52"/>
-        <v>14578433.333333334</v>
+        <v>17495100</v>
       </c>
       <c r="F103" s="29">
         <f t="shared" si="52"/>
-        <v>9993600</v>
+        <v>11993600</v>
       </c>
       <c r="G103" s="29">
         <f t="shared" si="52"/>
-        <v>7107984.615384615</v>
+        <v>8531061.538461538</v>
       </c>
       <c r="H103" s="29">
         <f t="shared" si="52"/>
-        <v>9750625</v>
+        <v>11703750</v>
       </c>
       <c r="I103" s="29">
         <f t="shared" si="52"/>
-        <v>6871555.1020408152</v>
+        <v>8249106.122448978</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
@@ -22237,32 +22237,32 @@
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C110" s="29">
-        <f t="shared" ref="C110:I116" si="54">IF(C69=$L$70,$L$70,$E$92/C69)</f>
-        <v>3162202.3809523811</v>
+        <f t="shared" ref="C110:I110" si="54">IF(C69=$L$70,$L$70,$E$92/C69)</f>
+        <v>3794642.8571428573</v>
       </c>
       <c r="D110" s="29">
         <f t="shared" si="54"/>
-        <v>22135416.666666664</v>
+        <v>26562500</v>
       </c>
       <c r="E110" s="29">
         <f t="shared" si="54"/>
-        <v>11362847.222222222</v>
+        <v>13635416.666666666</v>
       </c>
       <c r="F110" s="29">
         <f t="shared" si="54"/>
-        <v>3910590.2777777775</v>
+        <v>4692708.333333333</v>
       </c>
       <c r="G110" s="29">
         <f t="shared" si="54"/>
-        <v>2346354.1666666665</v>
+        <v>2815624.9999999995</v>
       </c>
       <c r="H110" s="29">
         <f t="shared" si="54"/>
-        <v>1466471.3541666667</v>
+        <v>1759765.625</v>
       </c>
       <c r="I110" s="29">
         <f t="shared" si="54"/>
-        <v>1303530.0925925926</v>
+        <v>1564236.1111111112</v>
       </c>
       <c r="K110" t="s">
         <v>18</v>
@@ -22290,19 +22290,19 @@
       </c>
       <c r="F111" s="29">
         <f t="shared" si="55"/>
-        <v>20432692.307692308</v>
+        <v>24519230.769230768</v>
       </c>
       <c r="G111" s="29">
         <f t="shared" si="55"/>
-        <v>15494791.666666666</v>
+        <v>18593750</v>
       </c>
       <c r="H111" s="29">
         <f t="shared" si="55"/>
-        <v>6500822.3684210526</v>
+        <v>7800986.8421052629</v>
       </c>
       <c r="I111" s="29">
         <f t="shared" si="55"/>
-        <v>1590661.3372093025</v>
+        <v>1908793.6046511629</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
@@ -22332,11 +22332,11 @@
       </c>
       <c r="H112" s="29">
         <f t="shared" si="56"/>
-        <v>2371651.7857142854</v>
+        <v>2845982.1428571427</v>
       </c>
       <c r="I112" s="29">
         <f t="shared" si="56"/>
-        <v>1328125</v>
+        <v>1593750</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.2">
@@ -22370,7 +22370,7 @@
       </c>
       <c r="I113" s="29">
         <f t="shared" si="57"/>
-        <v>9296875</v>
+        <v>11156250</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.2">
@@ -22380,31 +22380,31 @@
       </c>
       <c r="C114" s="29">
         <f t="shared" ref="C114:I114" si="58">IF(C73=$L$70,$L$70,$E$92/C73)</f>
-        <v>18110795.454545457</v>
+        <v>21732954.545454547</v>
       </c>
       <c r="D114" s="29">
         <f t="shared" si="58"/>
-        <v>53125000</v>
+        <v>63750000</v>
       </c>
       <c r="E114" s="29">
         <f t="shared" si="58"/>
-        <v>16098484.848484848</v>
+        <v>19318181.818181816</v>
       </c>
       <c r="F114" s="29">
         <f t="shared" si="58"/>
-        <v>10866477.272727273</v>
+        <v>13039772.727272728</v>
       </c>
       <c r="G114" s="29">
         <f t="shared" si="58"/>
-        <v>6439393.9393939395</v>
+        <v>7727272.7272727275</v>
       </c>
       <c r="H114" s="29">
         <f t="shared" si="58"/>
-        <v>4427083.333333333</v>
+        <v>5312500</v>
       </c>
       <c r="I114" s="29">
         <f t="shared" si="58"/>
-        <v>3311688.3116883119</v>
+        <v>3974025.9740259741</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.2">
@@ -22414,31 +22414,31 @@
       </c>
       <c r="C115" s="29">
         <f t="shared" ref="C115:I115" si="59">IF(C74=$L$70,$L$70,$E$92/C74)</f>
-        <v>26562500</v>
+        <v>31875000</v>
       </c>
       <c r="D115" s="29">
         <f t="shared" si="59"/>
-        <v>260312500.00000003</v>
+        <v>312375000</v>
       </c>
       <c r="E115" s="29">
         <f t="shared" si="59"/>
-        <v>157604166.66666666</v>
+        <v>189125000</v>
       </c>
       <c r="F115" s="29">
         <f t="shared" si="59"/>
-        <v>66572265.625000007</v>
+        <v>79886718.75</v>
       </c>
       <c r="G115" s="29">
         <f t="shared" si="59"/>
-        <v>35947916.666666672</v>
+        <v>43137500</v>
       </c>
       <c r="H115" s="29">
         <f t="shared" si="59"/>
-        <v>20217013.888888888</v>
+        <v>24260416.666666668</v>
       </c>
       <c r="I115" s="29">
         <f t="shared" si="59"/>
-        <v>14350649.350649349</v>
+        <v>17220779.220779218</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.2">
@@ -22448,31 +22448,31 @@
       </c>
       <c r="C116" s="29">
         <f t="shared" ref="C116:I116" si="60">IF(C75=$L$70,$L$70,$E$92/C75)</f>
-        <v>62500000</v>
+        <v>75000000</v>
       </c>
       <c r="D116" s="29">
         <f t="shared" si="60"/>
-        <v>27343750</v>
+        <v>32812500</v>
       </c>
       <c r="E116" s="29">
         <f t="shared" si="60"/>
-        <v>14583333.333333334</v>
+        <v>17500000</v>
       </c>
       <c r="F116" s="29">
         <f t="shared" si="60"/>
-        <v>10000000</v>
+        <v>12000000</v>
       </c>
       <c r="G116" s="29">
         <f t="shared" si="60"/>
-        <v>7115384.615384615</v>
+        <v>8538461.538461538</v>
       </c>
       <c r="H116" s="29">
         <f t="shared" si="60"/>
-        <v>9765625</v>
+        <v>11718750</v>
       </c>
       <c r="I116" s="29">
         <f t="shared" si="60"/>
-        <v>6887755.1020408152</v>
+        <v>8265306.122448978</v>
       </c>
     </row>
   </sheetData>
@@ -23020,13 +23020,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D11 C18:D24">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThanOrEqual">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>$K$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23085,7 +23085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
@@ -23101,7 +23101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
minor change in xlsx
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
@@ -19916,7 +19916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="J90" sqref="J90"/>
     </sheetView>
   </sheetViews>
@@ -23085,8 +23085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R140" sqref="R140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added TODOs, did sanity checks
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="85">
   <si>
     <t>Aktivität / Monat</t>
   </si>
@@ -272,10 +272,13 @@
     <t>PV (Planned Value)</t>
   </si>
   <si>
-    <t>TODO - materialkosten eigene formel</t>
+    <t>bac - ev</t>
   </si>
   <si>
-    <t>TODO materialkosten eigene formel</t>
+    <t xml:space="preserve">bac </t>
+  </si>
+  <si>
+    <t>ev</t>
   </si>
 </sst>
 </file>
@@ -575,118 +578,7 @@
     <cellStyle name="Text" xfId="4"/>
     <cellStyle name="Warning" xfId="11"/>
   </cellStyles>
-  <dxfs count="119">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="126">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -763,6 +655,117 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -915,6 +918,27 @@
       <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1017,13 +1041,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="SpBC" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="SpBC" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="118"/>
-      <tableStyleElement type="headerRow" dxfId="117"/>
-      <tableStyleElement type="totalRow" dxfId="116"/>
-      <tableStyleElement type="firstColumn" dxfId="115"/>
-      <tableStyleElement type="lastColumn" dxfId="114"/>
-      <tableStyleElement type="firstRowStripe" dxfId="113"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="112"/>
+      <tableStyleElement type="wholeTable" dxfId="125"/>
+      <tableStyleElement type="headerRow" dxfId="124"/>
+      <tableStyleElement type="totalRow" dxfId="123"/>
+      <tableStyleElement type="firstColumn" dxfId="122"/>
+      <tableStyleElement type="lastColumn" dxfId="121"/>
+      <tableStyleElement type="firstRowStripe" dxfId="120"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="119"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -9342,6 +9366,27 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76.766666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.514285714285691</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -9423,6 +9468,27 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>115.71428571428569</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -30382,7 +30448,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="EV" displayName="EV" ref="B3:I11" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PV" displayName="PV" ref="B3:I11" totalsRowCount="1">
   <autoFilter ref="B3:I10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -30395,31 +30461,31 @@
   </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" name="Posten" totalsRowLabel="Gesamt"/>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="111">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="118">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!B2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!B2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!B12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="110">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="117">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!C2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!C2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!C12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="109">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="116">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!D2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!D2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!D12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="108">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="115">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!E2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!E2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!E12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="107">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="114">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!F2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!F2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!F12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="106">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="113">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!G2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!G12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="105">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="112">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!H2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!H12)</totalsRowFormula>
     </tableColumn>
@@ -30432,35 +30498,35 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="EAC" displayName="EAC" ref="B109:I117" totalsRowCount="1">
   <autoFilter ref="B109:I116"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="14">
+    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="31">
       <calculatedColumnFormula>B97</calculatedColumnFormula>
       <totalsRowFormula>ETC[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="6">
+    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="29">
       <calculatedColumnFormula>IF(C69=$L$70,$L$70,'Budgetierte Kosten'!$P2/(C69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[1]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="5">
+    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="27">
       <calculatedColumnFormula>IF(D69=$L$70,$L$70,$E$92/(D69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[2]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="4">
+    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="25">
       <calculatedColumnFormula>IF(E69=$L$70,$L$70,$E$92/(E69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[3]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="3">
+    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="23">
       <calculatedColumnFormula>IF(F69=$L$70,$L$70,$E$92/(F69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[4]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="2">
+    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="21">
       <calculatedColumnFormula>IF(G69=$L$70,$L$70,$E$92/(G69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[5]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="1">
+    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="19">
       <calculatedColumnFormula>IF(H69=$L$70,$L$70,$E$92/(H69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[6]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="0">
+    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="17">
       <calculatedColumnFormula>IF(I69=$L$70,$L$70,$E$92/(I69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[7]]*1000)</totalsRowFormula>
     </tableColumn>
@@ -30476,20 +30542,20 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="47">
+    <tableColumn id="2" name="CPI" dataDxfId="10">
       <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="46">
+    <tableColumn id="3" name="SPI" dataDxfId="9">
       <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="45">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="44"/>
-    <tableColumn id="6" name="Status" dataDxfId="43">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="7"/>
+    <tableColumn id="6" name="Status" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Trend" dataDxfId="42">
+    <tableColumn id="7" name="Trend" dataDxfId="5">
       <calculatedColumnFormula>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -30504,19 +30570,19 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="41">
+    <tableColumn id="2" name="CPI" dataDxfId="4">
       <calculatedColumnFormula>Kennzahlen!H69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="40">
+    <tableColumn id="3" name="SPI" dataDxfId="3">
       <calculatedColumnFormula>Kennzahlen!H82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="39">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="2">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="38">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="1">
       <calculatedColumnFormula>F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Status" dataDxfId="37">
+    <tableColumn id="6" name="Status" dataDxfId="0">
       <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Trend"/>
@@ -30526,7 +30592,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="B29:I37" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="EV" displayName="EV" ref="B29:I37" totalsRowCount="1">
   <autoFilter ref="B29:I36">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -30538,37 +30604,37 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="104">
+    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="111">
       <calculatedColumnFormula>B17</calculatedColumnFormula>
       <totalsRowFormula>AC[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="103" totalsRowDxfId="28">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="110" totalsRowDxfId="109">
       <calculatedColumnFormula>C4*'Fertigstellungsgrad der Akt.'!B2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabelle2[1])</totalsRowFormula>
+      <totalsRowFormula>SUM(EV[1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="102" totalsRowDxfId="27">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="108" totalsRowDxfId="107">
       <calculatedColumnFormula>D4*'Fertigstellungsgrad der Akt.'!C2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabelle2[2])</totalsRowFormula>
+      <totalsRowFormula>SUM(EV[2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="101" totalsRowDxfId="26">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="106" totalsRowDxfId="105">
       <calculatedColumnFormula>E4*'Fertigstellungsgrad der Akt.'!D2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabelle2[3])</totalsRowFormula>
+      <totalsRowFormula>SUM(EV[3])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="100" totalsRowDxfId="25">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="104" totalsRowDxfId="103">
       <calculatedColumnFormula>F4*'Fertigstellungsgrad der Akt.'!E2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabelle2[4])</totalsRowFormula>
+      <totalsRowFormula>SUM(EV[4])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="99" totalsRowDxfId="24">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="102" totalsRowDxfId="101">
       <calculatedColumnFormula>G4*'Fertigstellungsgrad der Akt.'!F2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabelle2[5])</totalsRowFormula>
+      <totalsRowFormula>SUM(EV[5])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="98" totalsRowDxfId="23">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="100" totalsRowDxfId="99">
       <calculatedColumnFormula>H4*'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabelle2[6])</totalsRowFormula>
+      <totalsRowFormula>SUM(EV[6])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="97" totalsRowDxfId="22">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="98" totalsRowDxfId="97">
       <calculatedColumnFormula>I4*'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabelle2[7])</totalsRowFormula>
+      <totalsRowFormula>SUM(EV[7])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -30590,7 +30656,7 @@
   <tableColumns count="8">
     <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="96">
       <calculatedColumnFormula>B4</calculatedColumnFormula>
-      <totalsRowFormula>EV[[#Totals],[Posten]]</totalsRowFormula>
+      <totalsRowFormula>PV[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="95" totalsRowDxfId="94">
       <calculatedColumnFormula>'Tatsächliche Kosten'!B2*'Tatsächliche Kosten'!$B$15</calculatedColumnFormula>
@@ -30634,35 +30700,35 @@
   <tableColumns count="8">
     <tableColumn id="1" name="Posten" totalsRowFunction="custom">
       <calculatedColumnFormula>B30</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[Posten]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="81">
       <calculatedColumnFormula>C30-C17</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[1]]-AC[[#Totals],[1]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[1]]-AC[[#Totals],[1]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="80">
       <calculatedColumnFormula>D30-D17</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[2]]-AC[[#Totals],[2]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[2]]-AC[[#Totals],[2]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="79">
       <calculatedColumnFormula>E30-E17</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[3]]-AC[[#Totals],[3]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[3]]-AC[[#Totals],[3]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="78">
       <calculatedColumnFormula>F30-F17</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[4]]-AC[[#Totals],[4]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[4]]-AC[[#Totals],[4]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="77">
       <calculatedColumnFormula>G30-G17</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[5]]-AC[[#Totals],[5]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[5]]-AC[[#Totals],[5]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="76">
       <calculatedColumnFormula>H30-H17</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[6]]-AC[[#Totals],[6]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[6]]-AC[[#Totals],[6]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="75">
       <calculatedColumnFormula>I30-I17</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[7]]-AC[[#Totals],[7]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[7]]-AC[[#Totals],[7]]</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -30720,31 +30786,31 @@
     </tableColumn>
     <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="67">
       <calculatedColumnFormula>IF(C17=0,$L$70,C30/C17)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[1]]/AC[[#Totals],[1]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[1]]/AC[[#Totals],[1]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="66">
       <calculatedColumnFormula>IF(D17=0,$L$70,D30/D17)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[2]]/AC[[#Totals],[2]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[2]]/AC[[#Totals],[2]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="65">
       <calculatedColumnFormula>IF(E17=0,$L$70,E30/E17)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[3]]/AC[[#Totals],[3]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[3]]/AC[[#Totals],[3]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="64">
       <calculatedColumnFormula>IF(F17=0,$L$70,F30/F17)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[4]]/AC[[#Totals],[4]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[4]]/AC[[#Totals],[4]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="63">
       <calculatedColumnFormula>IF(G17=0,$L$70,G30/G17)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[5]]/AC[[#Totals],[5]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[5]]/AC[[#Totals],[5]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="62">
       <calculatedColumnFormula>IF(H17=0,$L$70,H30/H17)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[6]]/AC[[#Totals],[6]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[6]]/AC[[#Totals],[6]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="61">
       <calculatedColumnFormula>IF(I17=0,"-",I30/I17)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[7]]/AC[[#Totals],[7]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[7]]/AC[[#Totals],[7]]</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -30759,33 +30825,33 @@
       <calculatedColumnFormula>B69</calculatedColumnFormula>
       <totalsRowFormula>CPI[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="60">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="60" totalsRowDxfId="59">
       <calculatedColumnFormula>IF(C4=0,$L$70,C30/C4)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[1]]/EV[[#Totals],[1]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[1]]/PV[[#Totals],[1]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="59">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="58" totalsRowDxfId="57">
       <calculatedColumnFormula>IF(D4=0,$L$70,D30/D4)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[2]]/EV[[#Totals],[2]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[2]]/PV[[#Totals],[2]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="58">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="56" totalsRowDxfId="55">
       <calculatedColumnFormula>IF(E4=0,$L$70,E30/E4)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[3]]/EV[[#Totals],[3]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[3]]/PV[[#Totals],[3]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="57">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="54" totalsRowDxfId="53">
       <calculatedColumnFormula>IF(F4=0,$L$70,F30/F4)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[4]]/EV[[#Totals],[4]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[4]]/PV[[#Totals],[4]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="56">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="52" totalsRowDxfId="51">
       <calculatedColumnFormula>IF(G4=0,$L$70,G30/G4)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[5]]/EV[[#Totals],[5]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[5]]/PV[[#Totals],[5]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="55">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="50" totalsRowDxfId="49">
       <calculatedColumnFormula>IF(H4=0,$L$70,H30/H4)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[6]]/EV[[#Totals],[6]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[6]]/PV[[#Totals],[6]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="54">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="48" totalsRowDxfId="47">
       <calculatedColumnFormula>IF(I4=0,"-",I30/I4)</calculatedColumnFormula>
-      <totalsRowFormula>Tabelle2[[#Totals],[7]]/EV[[#Totals],[7]]</totalsRowFormula>
+      <totalsRowFormula>EV[[#Totals],[7]]/PV[[#Totals],[7]]</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -30812,37 +30878,37 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="ETC" displayName="ETC" ref="B96:I104" totalsRowCount="1">
   <autoFilter ref="B96:I103"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="36">
+    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="46">
       <calculatedColumnFormula>B82</calculatedColumnFormula>
       <totalsRowFormula>SPI[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="21">
+    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="44">
       <calculatedColumnFormula>IF(C69=$L$70,$L$70,('Budgetierte Kosten'!$P2-C30)/(C69*1000))</calculatedColumnFormula>
-      <totalsRowFormula>($E$92-Tabelle2[[#Totals],[1]])/(CPI[[#Totals],[1]]*1000)</totalsRowFormula>
+      <totalsRowFormula>($E$92-EV[[#Totals],[1]])/(CPI[[#Totals],[1]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="20">
+    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="42">
       <calculatedColumnFormula>IF(D69=$L$70,$L$70,($E$92-D30)/(D69*1000))</calculatedColumnFormula>
-      <totalsRowFormula>($E$92-Tabelle2[[#Totals],[2]])/(CPI[[#Totals],[2]]*1000)</totalsRowFormula>
+      <totalsRowFormula>($E$92-EV[[#Totals],[2]])/(CPI[[#Totals],[2]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="19">
+    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
       <calculatedColumnFormula>IF(E69=$L$70,$L$70,($E$92-E30)/(E69*1000))</calculatedColumnFormula>
-      <totalsRowFormula>($E$92-Tabelle2[[#Totals],[3]])/(CPI[[#Totals],[3]]*1000)</totalsRowFormula>
+      <totalsRowFormula>($E$92-EV[[#Totals],[3]])/(CPI[[#Totals],[3]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="18">
+    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="38">
       <calculatedColumnFormula>IF(F69=$L$70,$L$70,($E$92-F30)/(F69*1000))</calculatedColumnFormula>
-      <totalsRowFormula>($E$92-Tabelle2[[#Totals],[4]])/(CPI[[#Totals],[4]]*1000)</totalsRowFormula>
+      <totalsRowFormula>($E$92-EV[[#Totals],[4]])/(CPI[[#Totals],[4]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="17">
+    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="36">
       <calculatedColumnFormula>IF(G69=$L$70,$L$70,($E$92-G30)/(G69*1000))</calculatedColumnFormula>
-      <totalsRowFormula>($E$92-Tabelle2[[#Totals],[5]])/(CPI[[#Totals],[5]]*1000)</totalsRowFormula>
+      <totalsRowFormula>($E$92-EV[[#Totals],[5]])/(CPI[[#Totals],[5]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="16">
+    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>IF(H69=$L$70,$L$70,($E$92-H30)/(H69*1000))</calculatedColumnFormula>
-      <totalsRowFormula>($E$92-Tabelle2[[#Totals],[6]])/(CPI[[#Totals],[6]]*1000)</totalsRowFormula>
+      <totalsRowFormula>($E$92-EV[[#Totals],[6]])/(CPI[[#Totals],[6]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="15">
+    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="32">
       <calculatedColumnFormula>IF(I69=$L$70,$L$70,($E$92-I30)/(I69*1000))</calculatedColumnFormula>
-      <totalsRowFormula>($E$92-Tabelle2[[#Totals],[7]])/(CPI[[#Totals],[7]]*1000)</totalsRowFormula>
+      <totalsRowFormula>($E$92-EV[[#Totals],[7]])/(CPI[[#Totals],[7]]*1000)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="SpBC" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -31231,10 +31297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T117"/>
+  <dimension ref="A1:T124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J118" sqref="J118"/>
+      <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31573,6 +31639,10 @@
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
+      <c r="K13">
+        <f>SUM(PV[7])</f>
+        <v>723000</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
@@ -31851,7 +31921,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B24" t="str">
-        <f>EV[[#Totals],[Posten]]</f>
+        <f>PV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
       </c>
       <c r="C24" s="28">
@@ -31880,6 +31950,16 @@
       </c>
       <c r="I24" s="28">
         <f>SUM('Tatsächliche Kosten'!$B12:'Tatsächliche Kosten'!H12)</f>
+        <v>868750</v>
+      </c>
+      <c r="K24">
+        <f>SUM(AC[1])</f>
+        <v>83600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <f>SUM(AC[7])</f>
         <v>868750</v>
       </c>
     </row>
@@ -32164,31 +32244,31 @@
         <v>Gesamt</v>
       </c>
       <c r="C37" s="28">
-        <f>SUM(Tabelle2[1])</f>
+        <f>SUM(EV[1])</f>
         <v>83320</v>
       </c>
       <c r="D37" s="28">
-        <f>SUM(Tabelle2[2])</f>
+        <f>SUM(EV[2])</f>
         <v>30140</v>
       </c>
       <c r="E37" s="28">
-        <f>SUM(Tabelle2[3])</f>
+        <f>SUM(EV[3])</f>
         <v>72860</v>
       </c>
       <c r="F37" s="28">
-        <f>SUM(Tabelle2[4])</f>
+        <f>SUM(EV[4])</f>
         <v>139880</v>
       </c>
       <c r="G37" s="28">
-        <f>SUM(Tabelle2[5])</f>
+        <f>SUM(EV[5])</f>
         <v>209400</v>
       </c>
       <c r="H37" s="28">
-        <f>SUM(Tabelle2[6])</f>
+        <f>SUM(EV[6])</f>
         <v>349520</v>
       </c>
       <c r="I37" s="28">
-        <f>SUM(Tabelle2[7])</f>
+        <f>SUM(EV[7])</f>
         <v>597240</v>
       </c>
     </row>
@@ -32469,35 +32549,45 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B50" t="str">
-        <f>Tabelle2[[#Totals],[Posten]]</f>
+        <f>EV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
       </c>
       <c r="C50" s="28">
-        <f>Tabelle2[[#Totals],[1]]-AC[[#Totals],[1]]</f>
+        <f>EV[[#Totals],[1]]-AC[[#Totals],[1]]</f>
         <v>-280</v>
       </c>
       <c r="D50" s="28">
-        <f>Tabelle2[[#Totals],[2]]-AC[[#Totals],[2]]</f>
+        <f>EV[[#Totals],[2]]-AC[[#Totals],[2]]</f>
         <v>-318460</v>
       </c>
       <c r="E50" s="28">
-        <f>Tabelle2[[#Totals],[3]]-AC[[#Totals],[3]]</f>
+        <f>EV[[#Totals],[3]]-AC[[#Totals],[3]]</f>
         <v>-493040</v>
       </c>
       <c r="F50" s="28">
-        <f>Tabelle2[[#Totals],[4]]-AC[[#Totals],[4]]</f>
+        <f>EV[[#Totals],[4]]-AC[[#Totals],[4]]</f>
         <v>-538020</v>
       </c>
       <c r="G50" s="28">
-        <f>Tabelle2[[#Totals],[5]]-AC[[#Totals],[5]]</f>
+        <f>EV[[#Totals],[5]]-AC[[#Totals],[5]]</f>
         <v>-507750</v>
       </c>
       <c r="H50" s="28">
-        <f>Tabelle2[[#Totals],[6]]-AC[[#Totals],[6]]</f>
+        <f>EV[[#Totals],[6]]-AC[[#Totals],[6]]</f>
         <v>-437280</v>
       </c>
       <c r="I50" s="28">
-        <f>Tabelle2[[#Totals],[7]]-AC[[#Totals],[7]]</f>
+        <f>EV[[#Totals],[7]]-AC[[#Totals],[7]]</f>
+        <v>-271510</v>
+      </c>
+      <c r="K50">
+        <f>SUM(CV[1])</f>
+        <v>-280</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <f>SUM(CV[7])</f>
         <v>-271510</v>
       </c>
     </row>
@@ -32775,6 +32865,10 @@
         <f t="shared" si="5"/>
         <v>-8959.9999999999982</v>
       </c>
+      <c r="K62">
+        <f>SUM(SV[1])</f>
+        <v>3320</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B63" t="str">
@@ -32809,6 +32903,10 @@
         <f>SUM(SV[7])</f>
         <v>-125760</v>
       </c>
+      <c r="K63">
+        <f>SUM(SV[7])</f>
+        <v>-125760</v>
+      </c>
     </row>
     <row r="66" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A66" s="27" t="s">
@@ -33145,31 +33243,31 @@
         <v>Gesamt</v>
       </c>
       <c r="C76" s="29">
-        <f>Tabelle2[[#Totals],[1]]/AC[[#Totals],[1]]</f>
+        <f>EV[[#Totals],[1]]/AC[[#Totals],[1]]</f>
         <v>0.99665071770334923</v>
       </c>
       <c r="D76" s="29">
-        <f>Tabelle2[[#Totals],[2]]/AC[[#Totals],[2]]</f>
+        <f>EV[[#Totals],[2]]/AC[[#Totals],[2]]</f>
         <v>8.6460126219162367E-2</v>
       </c>
       <c r="E76" s="29">
-        <f>Tabelle2[[#Totals],[3]]/AC[[#Totals],[3]]</f>
+        <f>EV[[#Totals],[3]]/AC[[#Totals],[3]]</f>
         <v>0.12875066266124757</v>
       </c>
       <c r="F76" s="29">
-        <f>Tabelle2[[#Totals],[4]]/AC[[#Totals],[4]]</f>
+        <f>EV[[#Totals],[4]]/AC[[#Totals],[4]]</f>
         <v>0.20634311845404926</v>
       </c>
       <c r="G76" s="29">
-        <f>Tabelle2[[#Totals],[5]]/AC[[#Totals],[5]]</f>
+        <f>EV[[#Totals],[5]]/AC[[#Totals],[5]]</f>
         <v>0.29198912361430662</v>
       </c>
       <c r="H76" s="29">
-        <f>Tabelle2[[#Totals],[6]]/AC[[#Totals],[6]]</f>
+        <f>EV[[#Totals],[6]]/AC[[#Totals],[6]]</f>
         <v>0.44422979156075243</v>
       </c>
       <c r="I76" s="29">
-        <f>Tabelle2[[#Totals],[7]]/AC[[#Totals],[7]]</f>
+        <f>EV[[#Totals],[7]]/AC[[#Totals],[7]]</f>
         <v>0.68747050359712225</v>
       </c>
     </row>
@@ -33178,7 +33276,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>16</v>
       </c>
@@ -33204,7 +33302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B82" t="str">
         <f t="shared" ref="B82:B88" si="9">B69</f>
         <v>Anforderungsanalyse</v>
@@ -33247,7 +33345,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B83" t="str">
         <f t="shared" si="9"/>
         <v>Design und Architektur</v>
@@ -33281,7 +33379,7 @@
         <v>0.5488372093023256</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B84" t="str">
         <f t="shared" si="9"/>
         <v>Implementierung</v>
@@ -33315,7 +33413,7 @@
         <v>0.61250000000000004</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B85" t="str">
         <f t="shared" si="9"/>
         <v>Integration und Test</v>
@@ -33349,7 +33447,7 @@
         <v>3.9375</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B86" t="str">
         <f t="shared" si="9"/>
         <v>Projektmanagement</v>
@@ -33383,7 +33481,7 @@
         <v>0.9285714285714286</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B87" t="str">
         <f t="shared" si="9"/>
         <v>Puffer für unerwartetes</v>
@@ -33417,7 +33515,7 @@
         <v>1.0214285714285716</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B88" t="str">
         <f t="shared" si="9"/>
         <v>Materialkosten</v>
@@ -33451,41 +33549,41 @@
         <v>0.57333333333333347</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B89" t="str">
         <f>CPI[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
       </c>
       <c r="C89" s="29">
-        <f>Tabelle2[[#Totals],[1]]/EV[[#Totals],[1]]</f>
+        <f>EV[[#Totals],[1]]/PV[[#Totals],[1]]</f>
         <v>1.0415000000000001</v>
       </c>
       <c r="D89" s="29">
-        <f>Tabelle2[[#Totals],[2]]/EV[[#Totals],[2]]</f>
+        <f>EV[[#Totals],[2]]/PV[[#Totals],[2]]</f>
         <v>0.18837499999999999</v>
       </c>
       <c r="E89" s="29">
-        <f>Tabelle2[[#Totals],[3]]/EV[[#Totals],[3]]</f>
+        <f>EV[[#Totals],[3]]/PV[[#Totals],[3]]</f>
         <v>0.27915708812260537</v>
       </c>
       <c r="F89" s="29">
-        <f>Tabelle2[[#Totals],[4]]/EV[[#Totals],[4]]</f>
+        <f>EV[[#Totals],[4]]/PV[[#Totals],[4]]</f>
         <v>0.39965714285714288</v>
       </c>
       <c r="G89" s="29">
-        <f>Tabelle2[[#Totals],[5]]/EV[[#Totals],[5]]</f>
+        <f>EV[[#Totals],[5]]/PV[[#Totals],[5]]</f>
         <v>0.44839400428265525</v>
       </c>
       <c r="H89" s="29">
-        <f>Tabelle2[[#Totals],[6]]/EV[[#Totals],[6]]</f>
+        <f>EV[[#Totals],[6]]/PV[[#Totals],[6]]</f>
         <v>0.57867549668874174</v>
       </c>
       <c r="I89" s="29">
-        <f>Tabelle2[[#Totals],[7]]/EV[[#Totals],[7]]</f>
+        <f>EV[[#Totals],[7]]/PV[[#Totals],[7]]</f>
         <v>0.82605809128630703</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A92" s="33" t="s">
         <v>69</v>
       </c>
@@ -33493,12 +33591,12 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A94" s="27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>16</v>
       </c>
@@ -33523,8 +33621,20 @@
       <c r="I96" t="s">
         <v>79</v>
       </c>
+      <c r="N96" t="s">
+        <v>82</v>
+      </c>
+      <c r="O96" t="s">
+        <v>83</v>
+      </c>
+      <c r="P96" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B97" t="str">
         <f t="shared" ref="B97:B103" si="12">B82</f>
         <v>Anforderungsanalyse</v>
@@ -33563,8 +33673,24 @@
       <c r="L97" t="s">
         <v>68</v>
       </c>
+      <c r="N97">
+        <f>ETC[[#This Row],[7 '[k €']]]*I69</f>
+        <v>14.4</v>
+      </c>
+      <c r="O97">
+        <f>'Budgetierte Kosten'!P2</f>
+        <v>144000</v>
+      </c>
+      <c r="P97" s="28">
+        <f>I30</f>
+        <v>129600</v>
+      </c>
+      <c r="Q97" s="28">
+        <f>O97-P97</f>
+        <v>14400</v>
+      </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B98" t="str">
         <f t="shared" si="12"/>
         <v>Design und Architektur</v>
@@ -33597,8 +33723,24 @@
         <f>IF(I70=$L$70,$L$70,('Budgetierte Kosten'!$P3-I31)/(I70*1000))</f>
         <v>131.32499999999999</v>
       </c>
+      <c r="N98">
+        <f>ETC[[#This Row],[7 '[k €']]]*I70</f>
+        <v>141.6</v>
+      </c>
+      <c r="O98">
+        <f>'Budgetierte Kosten'!P3</f>
+        <v>236000</v>
+      </c>
+      <c r="P98" s="28">
+        <f t="shared" ref="P98:P103" si="13">I31</f>
+        <v>94400</v>
+      </c>
+      <c r="Q98" s="28">
+        <f t="shared" ref="Q98:Q103" si="14">O98-P98</f>
+        <v>141600</v>
+      </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B99" t="str">
         <f t="shared" si="12"/>
         <v>Implementierung</v>
@@ -33631,8 +33773,24 @@
         <f>IF(I71=$L$70,$L$70,('Budgetierte Kosten'!$P4-I32)/(I71*1000))</f>
         <v>127.50000000000001</v>
       </c>
+      <c r="N99">
+        <f>ETC[[#This Row],[7 '[k €']]]*I71</f>
+        <v>294</v>
+      </c>
+      <c r="O99">
+        <f>'Budgetierte Kosten'!P4</f>
+        <v>392000</v>
+      </c>
+      <c r="P99" s="28">
+        <f t="shared" si="13"/>
+        <v>98000</v>
+      </c>
+      <c r="Q99" s="28">
+        <f t="shared" si="14"/>
+        <v>294000</v>
+      </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B100" t="str">
         <f t="shared" si="12"/>
         <v>Integration und Test</v>
@@ -33665,8 +33823,24 @@
         <f>IF(I72=$L$70,$L$70,('Budgetierte Kosten'!$P5-I33)/(I72*1000))</f>
         <v>89.25</v>
       </c>
+      <c r="N100">
+        <f>ETC[[#This Row],[7 '[k €']]]*I72</f>
+        <v>189</v>
+      </c>
+      <c r="O100">
+        <f>'Budgetierte Kosten'!P5</f>
+        <v>252000</v>
+      </c>
+      <c r="P100" s="28">
+        <f t="shared" si="13"/>
+        <v>63000</v>
+      </c>
+      <c r="Q100" s="28">
+        <f t="shared" si="14"/>
+        <v>189000</v>
+      </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B101" t="str">
         <f t="shared" si="12"/>
         <v>Projektmanagement</v>
@@ -33699,8 +33873,24 @@
         <f>IF(I73=$L$70,$L$70,('Budgetierte Kosten'!$P6-I34)/(I73*1000))</f>
         <v>204.00000000000003</v>
       </c>
+      <c r="N101">
+        <f>ETC[[#This Row],[7 '[k €']]]*I73</f>
+        <v>143</v>
+      </c>
+      <c r="O101">
+        <f>'Budgetierte Kosten'!P6</f>
+        <v>286000</v>
+      </c>
+      <c r="P101" s="28">
+        <f t="shared" si="13"/>
+        <v>143000</v>
+      </c>
+      <c r="Q101" s="28">
+        <f t="shared" si="14"/>
+        <v>143000</v>
+      </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B102" t="str">
         <f t="shared" si="12"/>
         <v>Puffer für unerwartetes</v>
@@ -33733,63 +33923,119 @@
         <f>IF(I74=$L$70,$L$70,('Budgetierte Kosten'!$P7-I35)/(I74*1000))</f>
         <v>289.30909090909086</v>
       </c>
+      <c r="N102">
+        <f>ETC[[#This Row],[7 '[k €']]]*I74</f>
+        <v>46.8</v>
+      </c>
+      <c r="O102">
+        <f>'Budgetierte Kosten'!P7</f>
+        <v>104000</v>
+      </c>
+      <c r="P102" s="28">
+        <f t="shared" si="13"/>
+        <v>57200.000000000007</v>
+      </c>
+      <c r="Q102" s="28">
+        <f t="shared" si="14"/>
+        <v>46799.999999999993</v>
+      </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B103" t="str">
         <f t="shared" si="12"/>
         <v>Materialkosten</v>
       </c>
-      <c r="C103" s="29"/>
-      <c r="D103" s="29"/>
-      <c r="E103" s="29"/>
-      <c r="F103" s="29"/>
-      <c r="G103" s="29"/>
-      <c r="H103" s="29"/>
-      <c r="I103" s="29"/>
-      <c r="J103" t="s">
-        <v>82</v>
+      <c r="C103" s="29">
+        <f>IF(C75=$L$70,$L$70,('Budgetierte Kosten'!$O11-C36)/(C75*1000))</f>
+        <v>98</v>
+      </c>
+      <c r="D103" s="29">
+        <f>IF(D75=$L$70,$L$70,('Budgetierte Kosten'!$O11-D36)/(D75*1000))</f>
+        <v>84</v>
+      </c>
+      <c r="E103" s="29">
+        <f>IF(E75=$L$70,$L$70,('Budgetierte Kosten'!$O11-E36)/(E75*1000))</f>
+        <v>76.766666666666666</v>
+      </c>
+      <c r="F103" s="29">
+        <f>IF(F75=$L$70,$L$70,('Budgetierte Kosten'!$O11-F36)/(F75*1000))</f>
+        <v>73.599999999999994</v>
+      </c>
+      <c r="G103" s="29">
+        <f>IF(G75=$L$70,$L$70,('Budgetierte Kosten'!$O11-G36)/(G75*1000))</f>
+        <v>66.600000000000009</v>
+      </c>
+      <c r="H103" s="29">
+        <f>IF(H75=$L$70,$L$70,('Budgetierte Kosten'!$O11-H36)/(H75*1000))</f>
+        <v>110</v>
+      </c>
+      <c r="I103" s="29">
+        <f>IF(I75=$L$70,$L$70,('Budgetierte Kosten'!$O11-I36)/(I75*1000))</f>
+        <v>99.514285714285691</v>
+      </c>
+      <c r="N103">
+        <f>ETC[[#This Row],[7 '[k €']]]*I75</f>
+        <v>73.959999999999994</v>
+      </c>
+      <c r="O103">
+        <f>'Budgetierte Kosten'!O11</f>
+        <v>86000</v>
+      </c>
+      <c r="P103" s="28">
+        <f t="shared" si="13"/>
+        <v>12040.000000000002</v>
+      </c>
+      <c r="Q103" s="28">
+        <f t="shared" si="14"/>
+        <v>73960</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B104" t="str">
         <f>SPI[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
       </c>
       <c r="C104" s="29">
-        <f>($E$92-Tabelle2[[#Totals],[1]])/(CPI[[#Totals],[1]]*1000)</f>
+        <f>($E$92-EV[[#Totals],[1]])/(CPI[[#Totals],[1]]*1000)</f>
         <v>1421.4408065290447</v>
       </c>
       <c r="D104" s="29">
-        <f>($E$92-Tabelle2[[#Totals],[2]])/(CPI[[#Totals],[2]]*1000)</f>
+        <f>($E$92-EV[[#Totals],[2]])/(CPI[[#Totals],[2]]*1000)</f>
         <v>17000.437823490378</v>
       </c>
       <c r="E104" s="29">
-        <f>($E$92-Tabelle2[[#Totals],[3]])/(CPI[[#Totals],[3]]*1000)</f>
+        <f>($E$92-EV[[#Totals],[3]])/(CPI[[#Totals],[3]]*1000)</f>
         <v>11084.525473510843</v>
       </c>
       <c r="F104" s="29">
-        <f>($E$92-Tabelle2[[#Totals],[4]])/(CPI[[#Totals],[4]]*1000)</f>
+        <f>($E$92-EV[[#Totals],[4]])/(CPI[[#Totals],[4]]*1000)</f>
         <v>6591.5452387760943</v>
       </c>
       <c r="G104" s="29">
-        <f>($E$92-Tabelle2[[#Totals],[5]])/(CPI[[#Totals],[5]]*1000)</f>
+        <f>($E$92-EV[[#Totals],[5]])/(CPI[[#Totals],[5]]*1000)</f>
         <v>4420.0276504297999</v>
       </c>
       <c r="H104" s="29">
-        <f>($E$92-Tabelle2[[#Totals],[6]])/(CPI[[#Totals],[6]]*1000)</f>
+        <f>($E$92-EV[[#Totals],[6]])/(CPI[[#Totals],[6]]*1000)</f>
         <v>2589.8308079652097</v>
       </c>
       <c r="I104" s="29">
-        <f>($E$92-Tabelle2[[#Totals],[7]])/(CPI[[#Totals],[7]]*1000)</f>
+        <f>($E$92-EV[[#Totals],[7]])/(CPI[[#Totals],[7]]*1000)</f>
         <v>1313.1617942535665</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L106">
+        <f>SUM(ETC[7 '[k €']])</f>
+        <v>955.91504329004329</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A107" s="33" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>16</v>
       </c>
@@ -33815,9 +34061,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B110" t="str">
-        <f t="shared" ref="B110:B116" si="13">B97</f>
+        <f t="shared" ref="B110:B116" si="15">B97</f>
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C110" s="29">
@@ -33855,9 +34101,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B111" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Design und Architektur</v>
       </c>
       <c r="C111" s="29" t="str">
@@ -33889,9 +34135,9 @@
         <v>218.87499999999997</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B112" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Implementierung</v>
       </c>
       <c r="C112" s="29" t="str">
@@ -33923,9 +34169,9 @@
         <v>170.00000000000003</v>
       </c>
     </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B113" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Integration und Test</v>
       </c>
       <c r="C113" s="29" t="str">
@@ -33957,9 +34203,9 @@
         <v>119.00000000000001</v>
       </c>
     </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B114" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Projektmanagement</v>
       </c>
       <c r="C114" s="29">
@@ -33991,9 +34237,9 @@
         <v>408.00000000000006</v>
       </c>
     </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B115" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Puffer für unerwartetes</v>
       </c>
       <c r="C115" s="29">
@@ -34025,23 +34271,41 @@
         <v>642.90909090909088</v>
       </c>
     </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B116" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Materialkosten</v>
       </c>
-      <c r="C116" s="29"/>
-      <c r="D116" s="29"/>
-      <c r="E116" s="29"/>
-      <c r="F116" s="29"/>
-      <c r="G116" s="29"/>
-      <c r="H116" s="29"/>
-      <c r="I116" s="29"/>
-      <c r="J116" t="s">
-        <v>83</v>
+      <c r="C116" s="29">
+        <f>IF(C75=$L$70,$L$70,'Budgetierte Kosten'!$O11/(C75*1000))</f>
+        <v>100</v>
+      </c>
+      <c r="D116" s="29">
+        <f>IF(D75=$L$70,$L$70,'Budgetierte Kosten'!$O11/(D75*1000))</f>
+        <v>87.5</v>
+      </c>
+      <c r="E116" s="29">
+        <f>IF(E75=$L$70,$L$70,'Budgetierte Kosten'!$O11/(E75*1000))</f>
+        <v>81.666666666666671</v>
+      </c>
+      <c r="F116" s="29">
+        <f>IF(F75=$L$70,$L$70,'Budgetierte Kosten'!$O11/(F75*1000))</f>
+        <v>80</v>
+      </c>
+      <c r="G116" s="29">
+        <f>IF(G75=$L$70,$L$70,'Budgetierte Kosten'!$O11/(G75*1000))</f>
+        <v>74</v>
+      </c>
+      <c r="H116" s="29">
+        <f>IF(H75=$L$70,$L$70,'Budgetierte Kosten'!$O11/(H75*1000))</f>
+        <v>125</v>
+      </c>
+      <c r="I116" s="29">
+        <f>IF(I75=$L$70,$L$70,'Budgetierte Kosten'!$O11/(I75*1000))</f>
+        <v>115.71428571428569</v>
       </c>
     </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B117" t="str">
         <f>ETC[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -34073,6 +34337,56 @@
       <c r="I117" s="29">
         <f>$E$92/(CPI[[#Totals],[7]]*1000)</f>
         <v>2181.9117942535663</v>
+      </c>
+      <c r="L117">
+        <f>I110*I69</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="118" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L118">
+        <f t="shared" ref="L118:L124" si="16">I111*I70</f>
+        <v>235.99999999999997</v>
+      </c>
+    </row>
+    <row r="119" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L119">
+        <f t="shared" si="16"/>
+        <v>392.00000000000006</v>
+      </c>
+    </row>
+    <row r="120" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L120">
+        <f t="shared" si="16"/>
+        <v>252.00000000000003</v>
+      </c>
+    </row>
+    <row r="121" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L121">
+        <f t="shared" si="16"/>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="122" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L122">
+        <f t="shared" si="16"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="123" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L123">
+        <f t="shared" si="16"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="124" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L124">
+        <f t="shared" si="16"/>
+        <v>1499.9999999999998</v>
+      </c>
+      <c r="M124">
+        <f>SUM(L117:L123)</f>
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
@@ -34098,7 +34412,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -34674,13 +34988,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D12 C18:D25">
-    <cfRule type="cellIs" dxfId="53" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThanOrEqual">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>$K$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34739,7 +35053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="V170" sqref="V170"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
worked off some todos, added 1
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="86">
   <si>
     <t>Aktivität / Monat</t>
   </si>
@@ -280,6 +280,9 @@
   <si>
     <t>ev</t>
   </si>
+  <si>
+    <t>Kumulierte Kosten/Monat</t>
+  </si>
 </sst>
 </file>
 
@@ -292,7 +295,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -402,6 +405,19 @@
     </font>
     <font>
       <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -517,7 +533,7 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -558,6 +574,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent" xfId="13"/>
@@ -1296,7 +1314,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F564-4632-AB2D-5EEFF68B5D2E}"/>
@@ -1398,7 +1416,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F564-4632-AB2D-5EEFF68B5D2E}"/>
@@ -1500,7 +1518,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-F564-4632-AB2D-5EEFF68B5D2E}"/>
@@ -1713,7 +1731,7 @@
           <c:x val="0.75314559638378542"/>
           <c:y val="0.15941065313967398"/>
           <c:w val="0.22107702682997959"/>
-          <c:h val="0.22607804650946906"/>
+          <c:h val="0.30248527327388963"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -8550,7 +8568,7 @@
           <c:x val="0.75314559638378542"/>
           <c:y val="0.15941065313967398"/>
           <c:w val="0.22107702682997959"/>
-          <c:h val="0.22607804650946906"/>
+          <c:h val="0.3294176832568812"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -10402,7 +10420,7 @@
           <c:x val="0.75314559638378542"/>
           <c:y val="0.15941065313967398"/>
           <c:w val="0.22107702682997959"/>
-          <c:h val="0.22607804650946906"/>
+          <c:h val="0.31593837837264138"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -11710,6 +11728,905 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT"/>
+              <a:t>PV-Graph</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aktivität / Monat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$18:$N$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9597-48EC-BD6A-3314CA44469F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anforderungsanalyse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$19:$N$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>48000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>144000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>144000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9597-48EC-BD6A-3314CA44469F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Design und Architektur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$20:$N$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>152000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>172000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>192000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>208000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>224000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>236000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>236000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>236000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9597-48EC-BD6A-3314CA44469F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Implementierung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$21:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>208000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>304000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>352000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>380000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>392000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9597-48EC-BD6A-3314CA44469F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Integration und Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$22:$N$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>168000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>216000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>252000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9597-48EC-BD6A-3314CA44469F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Projektmanagement</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$23:$N$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>132000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>154000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>176000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>198000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>220000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>242000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>264000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>286000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-9597-48EC-BD6A-3314CA44469F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Puffer für unerwartetes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$24:$N$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>88000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>104000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-9597-48EC-BD6A-3314CA44469F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Materialkosten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$25:$N$25</c:f>
+              <c:numCache>
+                <c:formatCode>"€ "#,##0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>71000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>81000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-9597-48EC-BD6A-3314CA44469F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="363063576"/>
+        <c:axId val="363062264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="363063576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="363062264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="363062264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="363063576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -12283,7 +13200,7 @@
           <c:x val="0.75314559638378542"/>
           <c:y val="0.15941065313967398"/>
           <c:w val="0.22107702682997959"/>
-          <c:h val="0.22607804650946906"/>
+          <c:h val="0.30245931072788734"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -12925,7 +13842,7 @@
           <c:x val="0.75314559638378542"/>
           <c:y val="0.15941065313967398"/>
           <c:w val="0.22107702682997959"/>
-          <c:h val="0.22607804650946906"/>
+          <c:h val="0.35637570738596563"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -13567,7 +14484,7 @@
           <c:x val="0.75314559638378542"/>
           <c:y val="0.15941065313967398"/>
           <c:w val="0.22107702682997959"/>
-          <c:h val="0.22607804650946906"/>
+          <c:h val="0.32043151428357136"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -14209,7 +15126,7 @@
           <c:x val="0.75314559638378542"/>
           <c:y val="0.15941065313967398"/>
           <c:w val="0.22107702682997959"/>
-          <c:h val="0.22607804650946906"/>
+          <c:h val="0.32043140092089273"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -14851,7 +15768,7 @@
           <c:x val="0.75314559638378542"/>
           <c:y val="0.15941065313967398"/>
           <c:w val="0.22107702682997959"/>
-          <c:h val="0.22607804650946906"/>
+          <c:h val="0.33840349111389811"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -16868,6 +17785,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors25.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -25901,6 +26858,511 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style25.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -30444,6 +31906,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>156881</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>40340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>608852</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Diagramm 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DB5231E-5455-495C-8ADC-8E53F2F76325}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -31299,7 +32797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
@@ -35053,8 +36551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V170" sqref="V170"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35067,10 +36565,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView topLeftCell="B8" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -35722,10 +37220,531 @@
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
     </row>
+    <row r="17" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6</v>
+      </c>
+      <c r="H18" s="2">
+        <v>7</v>
+      </c>
+      <c r="I18" s="2">
+        <v>8</v>
+      </c>
+      <c r="J18" s="2">
+        <v>9</v>
+      </c>
+      <c r="K18" s="2">
+        <v>10</v>
+      </c>
+      <c r="L18" s="2">
+        <v>11</v>
+      </c>
+      <c r="M18" s="2">
+        <v>12</v>
+      </c>
+      <c r="N18" s="2">
+        <v>13</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <f>B2*$B$14</f>
+        <v>48000</v>
+      </c>
+      <c r="C19">
+        <f>C2*$B$14 + B19</f>
+        <v>96000</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:N19" si="5">D2*$B$14 + C19</f>
+        <v>144000</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="O19" s="6"/>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B24" si="6">B3*$B$14</f>
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:N24" si="7">C3*$B$14 + B20</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="7"/>
+        <v>20000</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>52000</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>96000</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="7"/>
+        <v>152000</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="7"/>
+        <v>172000</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>192000</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="7"/>
+        <v>208000</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="7"/>
+        <v>224000</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="7"/>
+        <v>236000</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="7"/>
+        <v>236000</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="7"/>
+        <v>236000</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="7"/>
+    </row>
+    <row r="21" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="7"/>
+        <v>24000</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="7"/>
+        <v>64000</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="7"/>
+        <v>112000</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="7"/>
+        <v>160000</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>208000</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="7"/>
+        <v>256000</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="7"/>
+        <v>304000</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="7"/>
+        <v>352000</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="7"/>
+        <v>380000</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="7"/>
+        <v>392000</v>
+      </c>
+      <c r="O21" s="6"/>
+      <c r="P21" s="7"/>
+    </row>
+    <row r="22" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="7"/>
+        <v>16000</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="7"/>
+        <v>40000</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="7"/>
+        <v>72000</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="7"/>
+        <v>120000</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="7"/>
+        <v>168000</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="7"/>
+        <v>216000</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="7"/>
+        <v>252000</v>
+      </c>
+      <c r="O22" s="6"/>
+      <c r="P22" s="7"/>
+    </row>
+    <row r="23" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="6"/>
+        <v>22000</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="7"/>
+        <v>44000</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="7"/>
+        <v>66000</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="7"/>
+        <v>88000</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="7"/>
+        <v>110000</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>132000</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="7"/>
+        <v>154000</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>176000</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="7"/>
+        <v>198000</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="7"/>
+        <v>220000</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="7"/>
+        <v>242000</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="7"/>
+        <v>264000</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="7"/>
+        <v>286000</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="7"/>
+    </row>
+    <row r="24" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="6"/>
+        <v>8000</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="7"/>
+        <v>16000</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="7"/>
+        <v>24000</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="7"/>
+        <v>40000</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="7"/>
+        <v>56000</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="7"/>
+        <v>64000</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="7"/>
+        <v>72000</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="7"/>
+        <v>80000</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="7"/>
+        <v>88000</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="7"/>
+        <v>96000</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="7"/>
+        <v>104000</v>
+      </c>
+      <c r="O24" s="6"/>
+      <c r="P24" s="7"/>
+    </row>
+    <row r="25" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="12">
+        <f>B11</f>
+        <v>2000</v>
+      </c>
+      <c r="C25" s="12">
+        <f>C11+B25</f>
+        <v>4000</v>
+      </c>
+      <c r="D25" s="12">
+        <f t="shared" ref="D25:N25" si="8">D11+C25</f>
+        <v>7000</v>
+      </c>
+      <c r="E25" s="12">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="F25" s="12">
+        <f t="shared" si="8"/>
+        <v>13000</v>
+      </c>
+      <c r="G25" s="12">
+        <f t="shared" si="8"/>
+        <v>16000</v>
+      </c>
+      <c r="H25" s="12">
+        <f t="shared" si="8"/>
+        <v>21000</v>
+      </c>
+      <c r="I25" s="12">
+        <f t="shared" si="8"/>
+        <v>26000</v>
+      </c>
+      <c r="J25" s="12">
+        <f t="shared" si="8"/>
+        <v>41000</v>
+      </c>
+      <c r="K25" s="12">
+        <f t="shared" si="8"/>
+        <v>56000</v>
+      </c>
+      <c r="L25" s="12">
+        <f t="shared" si="8"/>
+        <v>71000</v>
+      </c>
+      <c r="M25" s="12">
+        <f t="shared" si="8"/>
+        <v>81000</v>
+      </c>
+      <c r="N25" s="12">
+        <f t="shared" si="8"/>
+        <v>86000</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="8"/>
+    </row>
+    <row r="26" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="2">
+        <f>SUM(B19:B25)</f>
+        <v>80000</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" ref="C26:N26" si="9">SUM(C19:C25)</f>
+        <v>160000</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="9"/>
+        <v>261000</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="9"/>
+        <v>350000</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="9"/>
+        <v>467000</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="9"/>
+        <v>604000</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="9"/>
+        <v>723000</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="9"/>
+        <v>850000</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="9"/>
+        <v>991000</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="9"/>
+        <v>1148000</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="9"/>
+        <v>1301000</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="9"/>
+        <v>1417000</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="9"/>
+        <v>1500000</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
PV Graph vertical axis in k€
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -11799,7 +11799,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13324290961995416"/>
+          <c:y val="0.10404784261803769"/>
+          <c:w val="0.65907930234217649"/>
+          <c:h val="0.77138843919731881"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -12452,6 +12462,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Monat</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12516,7 +12581,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Planned-Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4317886747760441E-2"/>
+              <c:y val="0.37963470272608368"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0\ \k&quot;€&quot;" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12550,6 +12678,9 @@
         <c:crossAx val="363063576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -12561,6 +12692,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.81143317805227955"/>
+          <c:y val="9.756720357962588E-2"/>
+          <c:w val="0.17814270398610335"/>
+          <c:h val="0.37871547765859387"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13523,7 +13664,7 @@
             <c:numRef>
               <c:f>Kennzahlen!$C$57:$I$57</c:f>
               <c:numCache>
-                <c:formatCode>#.##0\ "$"</c:formatCode>
+                <c:formatCode>#,##0\ "€"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -14171,7 +14312,7 @@
             <c:numRef>
               <c:f>Kennzahlen!$C$58:$I$58</c:f>
               <c:numCache>
-                <c:formatCode>#.##0\ "$"</c:formatCode>
+                <c:formatCode>#,##0\ "€"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -14819,7 +14960,7 @@
             <c:numRef>
               <c:f>Kennzahlen!$C$59:$I$59</c:f>
               <c:numCache>
-                <c:formatCode>#.##0\ "$"</c:formatCode>
+                <c:formatCode>#,##0\ "€"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -16109,7 +16250,7 @@
             <c:numRef>
               <c:f>Kennzahlen!$C$60:$I$60</c:f>
               <c:numCache>
-                <c:formatCode>#.##0\ "$"</c:formatCode>
+                <c:formatCode>#,##0\ "€"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>880</c:v>
@@ -16757,7 +16898,7 @@
             <c:numRef>
               <c:f>Kennzahlen!$C$61:$I$61</c:f>
               <c:numCache>
-                <c:formatCode>#.##0\ "$"</c:formatCode>
+                <c:formatCode>#,##0\ "€"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>320</c:v>
@@ -17405,7 +17546,7 @@
             <c:numRef>
               <c:f>Kennzahlen!$C$62:$I$62</c:f>
               <c:numCache>
-                <c:formatCode>#.##0\ "$"</c:formatCode>
+                <c:formatCode>#,##0\ "€"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>-280</c:v>
@@ -18053,7 +18194,7 @@
             <c:numRef>
               <c:f>Kennzahlen!$C$63:$I$63</c:f>
               <c:numCache>
-                <c:formatCode>#.##0\ "$"</c:formatCode>
+                <c:formatCode>#,##0\ "€"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3320</c:v>
@@ -41541,15 +41682,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>470645</xdr:colOff>
+      <xdr:colOff>22970</xdr:colOff>
       <xdr:row>161</xdr:row>
-      <xdr:rowOff>40340</xdr:rowOff>
+      <xdr:rowOff>2241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>160616</xdr:colOff>
-      <xdr:row>189</xdr:row>
-      <xdr:rowOff>33617</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -46550,8 +46691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI149" sqref="AI149"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O170" sqref="O170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added RAG-Gesamtprozentberechnung, linie in Anforderungsanalyse ungegelaettet
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sack\Christian\A\Studium\4 - Semester\SpBC\Übungen\swpbc\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Karriere\TU\2017SS\SwPBC\swpbc\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="89">
   <si>
     <t>Aktivität / Monat</t>
   </si>
@@ -283,19 +283,29 @@
   <si>
     <t>Kumulierte Kosten/Monat</t>
   </si>
+  <si>
+    <t>BAC-Anteil</t>
+  </si>
+  <si>
+    <t>relativer BAC-Anteil</t>
+  </si>
+  <si>
+    <t>Fertigstellungsgrad in Relation zum beigetragenen BAC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="6">
+    <numFmt numFmtId="5" formatCode="&quot;€&quot;\ #,##0;\-&quot;€&quot;\ #,##0"/>
     <numFmt numFmtId="164" formatCode="&quot;€ &quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;€ &quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     <numFmt numFmtId="167" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -421,6 +431,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -533,7 +549,7 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -576,6 +592,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="5" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent" xfId="13"/>
@@ -598,39 +617,10 @@
   </cellStyles>
   <dxfs count="126">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <fill>
@@ -673,6 +663,35 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1314,7 +1333,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F564-4632-AB2D-5EEFF68B5D2E}"/>
@@ -1416,7 +1435,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F564-4632-AB2D-5EEFF68B5D2E}"/>
@@ -1518,7 +1537,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-F564-4632-AB2D-5EEFF68B5D2E}"/>
@@ -11920,7 +11939,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$19:$N$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>48000</c:v>
@@ -11998,7 +12017,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$20:$N$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -12076,7 +12095,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$21:$N$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -12154,7 +12173,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$22:$N$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -12232,7 +12251,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$23:$N$23</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>22000</c:v>
@@ -12312,7 +12331,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$24:$N$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>8000</c:v>
@@ -12392,7 +12411,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$25:$N$25</c:f>
               <c:numCache>
-                <c:formatCode>"€ "#,##0</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
@@ -42133,20 +42152,20 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="10">
+    <tableColumn id="2" name="CPI" dataDxfId="16">
       <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="9">
+    <tableColumn id="3" name="SPI" dataDxfId="15">
       <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="1">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="7"/>
-    <tableColumn id="6" name="Status" dataDxfId="6">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="14"/>
+    <tableColumn id="6" name="Status" dataDxfId="13">
       <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Trend" dataDxfId="5">
+    <tableColumn id="7" name="Trend" dataDxfId="12">
       <calculatedColumnFormula>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -42161,19 +42180,19 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="4">
+    <tableColumn id="2" name="CPI" dataDxfId="11">
       <calculatedColumnFormula>Kennzahlen!H69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="3">
+    <tableColumn id="3" name="SPI" dataDxfId="10">
       <calculatedColumnFormula>Kennzahlen!H82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="2">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="0">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="1">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="9">
       <calculatedColumnFormula>F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Status" dataDxfId="0">
+    <tableColumn id="6" name="Status" dataDxfId="8">
       <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Trend"/>
@@ -42890,8 +42909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U43" sqref="U43"/>
+    <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L119" sqref="L119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46049,8 +46068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46358,8 +46377,8 @@
         <v>0.82605809128630703</v>
       </c>
       <c r="E12" s="30">
-        <f>'Fertigstellungsgrad der Akt.'!H9</f>
-        <v>0</v>
+        <f>'Fertigstellungsgrad der Akt.'!H20</f>
+        <v>0.39816000000000001</v>
       </c>
       <c r="F12" s="31">
         <f>'Budgetierte Kosten'!P11/1000</f>
@@ -46612,8 +46631,8 @@
         <v>0.57867549668874174</v>
       </c>
       <c r="E25" s="30">
-        <f>'Fertigstellungsgrad der Akt.'!G9</f>
-        <v>0</v>
+        <f>'Fertigstellungsgrad der Akt.'!G20</f>
+        <v>0.23301333333333335</v>
       </c>
       <c r="F25" s="31">
         <f t="shared" si="0"/>
@@ -46626,13 +46645,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D12 C18:D25">
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="greaterThanOrEqual">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="lessThan">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="lessThan">
       <formula>$K$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46691,7 +46710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O170" sqref="O170"/>
     </sheetView>
   </sheetViews>
@@ -46707,8 +46726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -46717,7 +46736,10 @@
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="13" width="9.42578125" customWidth="1"/>
+    <col min="5" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" customWidth="1"/>
@@ -46767,8 +46789,12 @@
         <v>13</v>
       </c>
       <c r="O1" s="2"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4"/>
+      <c r="P1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="2" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -46821,6 +46847,10 @@
         <f t="shared" ref="P2:P8" si="1">O2*$B$14</f>
         <v>144000</v>
       </c>
+      <c r="Q2">
+        <f>P2/$P$11</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -46873,6 +46903,10 @@
         <f t="shared" si="1"/>
         <v>236000</v>
       </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q7" si="2">P3/$P$11</f>
+        <v>0.15733333333333333</v>
+      </c>
     </row>
     <row r="4" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -46925,6 +46959,10 @@
         <f t="shared" si="1"/>
         <v>392000</v>
       </c>
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>0.26133333333333331</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -46977,6 +47015,10 @@
         <f t="shared" si="1"/>
         <v>252000</v>
       </c>
+      <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>0.16800000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -47029,6 +47071,10 @@
         <f t="shared" si="1"/>
         <v>286000</v>
       </c>
+      <c r="Q6">
+        <f t="shared" si="2"/>
+        <v>0.19066666666666668</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -47081,65 +47127,69 @@
         <f t="shared" si="1"/>
         <v>104000</v>
       </c>
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>6.933333333333333E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" ref="B8:O8" si="2">SUM(B2:B7)</f>
+        <f t="shared" ref="B8:O8" si="3">SUM(B2:B7)</f>
         <v>975</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>975</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1225</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1075</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1425</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1675</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1425</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1525</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1575</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1775</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1725</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1325</v>
       </c>
       <c r="N8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>975</v>
       </c>
       <c r="O8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17675</v>
       </c>
       <c r="P8" s="8">
@@ -47156,55 +47206,55 @@
         <v>8</v>
       </c>
       <c r="B10" s="12">
-        <f t="shared" ref="B10:N10" si="3">B8*$B$14</f>
+        <f t="shared" ref="B10:N10" si="4">B8*$B$14</f>
         <v>78000</v>
       </c>
       <c r="C10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78000</v>
       </c>
       <c r="D10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98000</v>
       </c>
       <c r="E10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>86000</v>
       </c>
       <c r="F10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>114000</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>134000</v>
       </c>
       <c r="H10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>114000</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>122000</v>
       </c>
       <c r="J10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126000</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>142000</v>
       </c>
       <c r="L10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>138000</v>
       </c>
       <c r="M10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>106000</v>
       </c>
       <c r="N10" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78000</v>
       </c>
       <c r="O10" s="2" t="s">
@@ -47263,61 +47313,65 @@
         <f>O11+P8</f>
         <v>1500000</v>
       </c>
+      <c r="Q11">
+        <f>O11/$P$11</f>
+        <v>5.7333333333333333E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="14">
-        <f t="shared" ref="B12:N12" si="4">SUM(B10:B11)</f>
+        <f t="shared" ref="B12:N12" si="5">SUM(B10:B11)</f>
         <v>80000</v>
       </c>
       <c r="C12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80000</v>
       </c>
       <c r="D12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>101000</v>
       </c>
       <c r="E12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89000</v>
       </c>
       <c r="F12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>117000</v>
       </c>
       <c r="G12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>137000</v>
       </c>
       <c r="H12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119000</v>
       </c>
       <c r="I12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>127000</v>
       </c>
       <c r="J12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>141000</v>
       </c>
       <c r="K12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>157000</v>
       </c>
       <c r="L12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>153000</v>
       </c>
       <c r="M12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>116000</v>
       </c>
       <c r="N12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83000</v>
       </c>
       <c r="P12" s="3"/>
@@ -47415,56 +47469,56 @@
       <c r="A19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="39">
         <f>B2*$B$14</f>
         <v>48000</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="39">
         <f>C2*$B$14 + B19</f>
         <v>96000</v>
       </c>
-      <c r="D19">
-        <f t="shared" ref="D19:N19" si="5">D2*$B$14 + C19</f>
+      <c r="D19" s="39">
+        <f t="shared" ref="D19:N19" si="6">D2*$B$14 + C19</f>
         <v>144000</v>
       </c>
-      <c r="E19">
-        <f t="shared" si="5"/>
+      <c r="E19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="5"/>
+      <c r="F19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
-      <c r="G19">
-        <f t="shared" si="5"/>
+      <c r="G19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="5"/>
+      <c r="H19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="5"/>
+      <c r="I19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="5"/>
+      <c r="J19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="5"/>
+      <c r="K19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
-      <c r="L19">
-        <f t="shared" si="5"/>
+      <c r="L19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
-      <c r="M19">
-        <f t="shared" si="5"/>
+      <c r="M19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
-      <c r="N19">
-        <f t="shared" si="5"/>
+      <c r="N19" s="39">
+        <f t="shared" si="6"/>
         <v>144000</v>
       </c>
       <c r="O19" s="6"/>
@@ -47474,56 +47528,56 @@
       <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B20">
-        <f t="shared" ref="B20:B24" si="6">B3*$B$14</f>
+      <c r="B20" s="39">
+        <f t="shared" ref="B20:B24" si="7">B3*$B$14</f>
         <v>0</v>
       </c>
-      <c r="C20">
-        <f t="shared" ref="C20:N24" si="7">C3*$B$14 + B20</f>
+      <c r="C20" s="39">
+        <f t="shared" ref="C20:N24" si="8">C3*$B$14 + B20</f>
         <v>0</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="7"/>
+      <c r="D20" s="39">
+        <f t="shared" si="8"/>
         <v>20000</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="7"/>
+      <c r="E20" s="39">
+        <f t="shared" si="8"/>
         <v>52000</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="7"/>
+      <c r="F20" s="39">
+        <f t="shared" si="8"/>
         <v>96000</v>
       </c>
-      <c r="G20">
-        <f t="shared" si="7"/>
+      <c r="G20" s="39">
+        <f t="shared" si="8"/>
         <v>152000</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="7"/>
+      <c r="H20" s="39">
+        <f t="shared" si="8"/>
         <v>172000</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="7"/>
+      <c r="I20" s="39">
+        <f t="shared" si="8"/>
         <v>192000</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="7"/>
+      <c r="J20" s="39">
+        <f t="shared" si="8"/>
         <v>208000</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="7"/>
+      <c r="K20" s="39">
+        <f t="shared" si="8"/>
         <v>224000</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="7"/>
+      <c r="L20" s="39">
+        <f t="shared" si="8"/>
         <v>236000</v>
       </c>
-      <c r="M20">
-        <f t="shared" si="7"/>
+      <c r="M20" s="39">
+        <f t="shared" si="8"/>
         <v>236000</v>
       </c>
-      <c r="N20">
-        <f t="shared" si="7"/>
+      <c r="N20" s="39">
+        <f t="shared" si="8"/>
         <v>236000</v>
       </c>
       <c r="O20" s="6"/>
@@ -47533,56 +47587,56 @@
       <c r="A21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B21">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="39">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="7"/>
+      <c r="C21" s="39">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="7"/>
+      <c r="D21" s="39">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="39">
+        <f t="shared" si="8"/>
         <v>24000</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="7"/>
+      <c r="F21" s="39">
+        <f t="shared" si="8"/>
         <v>64000</v>
       </c>
-      <c r="G21">
-        <f t="shared" si="7"/>
+      <c r="G21" s="39">
+        <f t="shared" si="8"/>
         <v>112000</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="7"/>
+      <c r="H21" s="39">
+        <f t="shared" si="8"/>
         <v>160000</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="7"/>
+      <c r="I21" s="39">
+        <f t="shared" si="8"/>
         <v>208000</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="7"/>
+      <c r="J21" s="39">
+        <f t="shared" si="8"/>
         <v>256000</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="7"/>
+      <c r="K21" s="39">
+        <f t="shared" si="8"/>
         <v>304000</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="7"/>
+      <c r="L21" s="39">
+        <f t="shared" si="8"/>
         <v>352000</v>
       </c>
-      <c r="M21">
-        <f t="shared" si="7"/>
+      <c r="M21" s="39">
+        <f t="shared" si="8"/>
         <v>380000</v>
       </c>
-      <c r="N21">
-        <f t="shared" si="7"/>
+      <c r="N21" s="39">
+        <f t="shared" si="8"/>
         <v>392000</v>
       </c>
       <c r="O21" s="6"/>
@@ -47592,56 +47646,56 @@
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B22">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="39">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="7"/>
+      <c r="C22" s="39">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="7"/>
+      <c r="D22" s="39">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="7"/>
+      <c r="E22" s="39">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G22">
-        <f t="shared" si="7"/>
+      <c r="F22" s="39">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="7"/>
+      <c r="G22" s="39">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="39">
+        <f t="shared" si="8"/>
         <v>16000</v>
       </c>
-      <c r="I22">
-        <f t="shared" si="7"/>
+      <c r="I22" s="39">
+        <f t="shared" si="8"/>
         <v>40000</v>
       </c>
-      <c r="J22">
-        <f t="shared" si="7"/>
+      <c r="J22" s="39">
+        <f t="shared" si="8"/>
         <v>72000</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="7"/>
+      <c r="K22" s="39">
+        <f t="shared" si="8"/>
         <v>120000</v>
       </c>
-      <c r="L22">
-        <f t="shared" si="7"/>
+      <c r="L22" s="39">
+        <f t="shared" si="8"/>
         <v>168000</v>
       </c>
-      <c r="M22">
-        <f t="shared" si="7"/>
+      <c r="M22" s="39">
+        <f t="shared" si="8"/>
         <v>216000</v>
       </c>
-      <c r="N22">
-        <f t="shared" si="7"/>
+      <c r="N22" s="39">
+        <f t="shared" si="8"/>
         <v>252000</v>
       </c>
       <c r="O22" s="6"/>
@@ -47651,56 +47705,56 @@
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B23">
-        <f t="shared" si="6"/>
+      <c r="B23" s="39">
+        <f t="shared" si="7"/>
         <v>22000</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="7"/>
+      <c r="C23" s="39">
+        <f t="shared" si="8"/>
         <v>44000</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="7"/>
+      <c r="D23" s="39">
+        <f t="shared" si="8"/>
         <v>66000</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="7"/>
+      <c r="E23" s="39">
+        <f t="shared" si="8"/>
         <v>88000</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="7"/>
+      <c r="F23" s="39">
+        <f t="shared" si="8"/>
         <v>110000</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="7"/>
+      <c r="G23" s="39">
+        <f t="shared" si="8"/>
         <v>132000</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="7"/>
+      <c r="H23" s="39">
+        <f t="shared" si="8"/>
         <v>154000</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="7"/>
+      <c r="I23" s="39">
+        <f t="shared" si="8"/>
         <v>176000</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="7"/>
+      <c r="J23" s="39">
+        <f t="shared" si="8"/>
         <v>198000</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="7"/>
+      <c r="K23" s="39">
+        <f t="shared" si="8"/>
         <v>220000</v>
       </c>
-      <c r="L23">
-        <f t="shared" si="7"/>
+      <c r="L23" s="39">
+        <f t="shared" si="8"/>
         <v>242000</v>
       </c>
-      <c r="M23">
-        <f t="shared" si="7"/>
+      <c r="M23" s="39">
+        <f t="shared" si="8"/>
         <v>264000</v>
       </c>
-      <c r="N23">
-        <f t="shared" si="7"/>
+      <c r="N23" s="39">
+        <f t="shared" si="8"/>
         <v>286000</v>
       </c>
       <c r="O23" s="6"/>
@@ -47710,56 +47764,56 @@
       <c r="A24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B24">
-        <f t="shared" si="6"/>
+      <c r="B24" s="39">
+        <f t="shared" si="7"/>
         <v>8000</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="7"/>
+      <c r="C24" s="39">
+        <f t="shared" si="8"/>
         <v>16000</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="7"/>
+      <c r="D24" s="39">
+        <f t="shared" si="8"/>
         <v>24000</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="7"/>
+      <c r="E24" s="39">
+        <f t="shared" si="8"/>
         <v>32000</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="7"/>
+      <c r="F24" s="39">
+        <f t="shared" si="8"/>
         <v>40000</v>
       </c>
-      <c r="G24">
-        <f t="shared" si="7"/>
+      <c r="G24" s="39">
+        <f t="shared" si="8"/>
         <v>48000</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="7"/>
+      <c r="H24" s="39">
+        <f t="shared" si="8"/>
         <v>56000</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="7"/>
+      <c r="I24" s="39">
+        <f t="shared" si="8"/>
         <v>64000</v>
       </c>
-      <c r="J24">
-        <f t="shared" si="7"/>
+      <c r="J24" s="39">
+        <f t="shared" si="8"/>
         <v>72000</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="7"/>
+      <c r="K24" s="39">
+        <f t="shared" si="8"/>
         <v>80000</v>
       </c>
-      <c r="L24">
-        <f t="shared" si="7"/>
+      <c r="L24" s="39">
+        <f t="shared" si="8"/>
         <v>88000</v>
       </c>
-      <c r="M24">
-        <f t="shared" si="7"/>
+      <c r="M24" s="39">
+        <f t="shared" si="8"/>
         <v>96000</v>
       </c>
-      <c r="N24">
-        <f t="shared" si="7"/>
+      <c r="N24" s="39">
+        <f t="shared" si="8"/>
         <v>104000</v>
       </c>
       <c r="O24" s="6"/>
@@ -47769,56 +47823,56 @@
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="39">
         <f>B11</f>
         <v>2000</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="39">
         <f>C11+B25</f>
         <v>4000</v>
       </c>
-      <c r="D25" s="12">
-        <f t="shared" ref="D25:N25" si="8">D11+C25</f>
+      <c r="D25" s="39">
+        <f t="shared" ref="D25:N25" si="9">D11+C25</f>
         <v>7000</v>
       </c>
-      <c r="E25" s="12">
-        <f t="shared" si="8"/>
+      <c r="E25" s="39">
+        <f t="shared" si="9"/>
         <v>10000</v>
       </c>
-      <c r="F25" s="12">
-        <f t="shared" si="8"/>
+      <c r="F25" s="39">
+        <f t="shared" si="9"/>
         <v>13000</v>
       </c>
-      <c r="G25" s="12">
-        <f t="shared" si="8"/>
+      <c r="G25" s="39">
+        <f t="shared" si="9"/>
         <v>16000</v>
       </c>
-      <c r="H25" s="12">
-        <f t="shared" si="8"/>
+      <c r="H25" s="39">
+        <f t="shared" si="9"/>
         <v>21000</v>
       </c>
-      <c r="I25" s="12">
-        <f t="shared" si="8"/>
+      <c r="I25" s="39">
+        <f t="shared" si="9"/>
         <v>26000</v>
       </c>
-      <c r="J25" s="12">
-        <f t="shared" si="8"/>
+      <c r="J25" s="39">
+        <f t="shared" si="9"/>
         <v>41000</v>
       </c>
-      <c r="K25" s="12">
-        <f t="shared" si="8"/>
+      <c r="K25" s="39">
+        <f t="shared" si="9"/>
         <v>56000</v>
       </c>
-      <c r="L25" s="12">
-        <f t="shared" si="8"/>
+      <c r="L25" s="39">
+        <f t="shared" si="9"/>
         <v>71000</v>
       </c>
-      <c r="M25" s="12">
-        <f t="shared" si="8"/>
+      <c r="M25" s="39">
+        <f t="shared" si="9"/>
         <v>81000</v>
       </c>
-      <c r="N25" s="12">
-        <f t="shared" si="8"/>
+      <c r="N25" s="39">
+        <f t="shared" si="9"/>
         <v>86000</v>
       </c>
       <c r="O25" s="2"/>
@@ -47828,56 +47882,56 @@
       <c r="A26" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="40">
         <f>SUM(B19:B25)</f>
         <v>80000</v>
       </c>
-      <c r="C26" s="2">
-        <f t="shared" ref="C26:N26" si="9">SUM(C19:C25)</f>
+      <c r="C26" s="40">
+        <f t="shared" ref="C26:N26" si="10">SUM(C19:C25)</f>
         <v>160000</v>
       </c>
-      <c r="D26" s="2">
-        <f t="shared" si="9"/>
+      <c r="D26" s="40">
+        <f t="shared" si="10"/>
         <v>261000</v>
       </c>
-      <c r="E26" s="2">
-        <f t="shared" si="9"/>
+      <c r="E26" s="40">
+        <f t="shared" si="10"/>
         <v>350000</v>
       </c>
-      <c r="F26" s="2">
-        <f t="shared" si="9"/>
+      <c r="F26" s="40">
+        <f t="shared" si="10"/>
         <v>467000</v>
       </c>
-      <c r="G26" s="2">
-        <f t="shared" si="9"/>
+      <c r="G26" s="40">
+        <f t="shared" si="10"/>
         <v>604000</v>
       </c>
-      <c r="H26" s="2">
-        <f t="shared" si="9"/>
+      <c r="H26" s="40">
+        <f t="shared" si="10"/>
         <v>723000</v>
       </c>
-      <c r="I26" s="2">
-        <f t="shared" si="9"/>
+      <c r="I26" s="40">
+        <f t="shared" si="10"/>
         <v>850000</v>
       </c>
-      <c r="J26" s="2">
-        <f t="shared" si="9"/>
+      <c r="J26" s="40">
+        <f t="shared" si="10"/>
         <v>991000</v>
       </c>
-      <c r="K26" s="2">
-        <f t="shared" si="9"/>
+      <c r="K26" s="40">
+        <f t="shared" si="10"/>
         <v>1148000</v>
       </c>
-      <c r="L26" s="2">
-        <f t="shared" si="9"/>
+      <c r="L26" s="40">
+        <f>SUM(L19:L25)</f>
         <v>1301000</v>
       </c>
-      <c r="M26" s="2">
-        <f t="shared" si="9"/>
+      <c r="M26" s="40">
+        <f t="shared" si="10"/>
         <v>1417000</v>
       </c>
-      <c r="N26" s="2">
-        <f t="shared" si="9"/>
+      <c r="N26" s="40">
+        <f t="shared" si="10"/>
         <v>1500000</v>
       </c>
     </row>
@@ -48267,10 +48321,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -48507,8 +48561,332 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="str">
+        <f>'Budgetierte Kosten'!A2</f>
+        <v>Anforderungsanalyse</v>
+      </c>
+      <c r="B13" s="26">
+        <f>B2*'Budgetierte Kosten'!$Q2</f>
+        <v>3.3599999999999998E-2</v>
+      </c>
+      <c r="C13" s="26">
+        <f>C2*'Budgetierte Kosten'!$Q2</f>
+        <v>4.8000000000000004E-3</v>
+      </c>
+      <c r="D13" s="26">
+        <f>D2*'Budgetierte Kosten'!$Q2</f>
+        <v>9.6000000000000009E-3</v>
+      </c>
+      <c r="E13" s="26">
+        <f>E2*'Budgetierte Kosten'!$Q2</f>
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="F13" s="26">
+        <f>F2*'Budgetierte Kosten'!$Q2</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="G13" s="26">
+        <f>G2*'Budgetierte Kosten'!$Q2</f>
+        <v>7.6800000000000007E-2</v>
+      </c>
+      <c r="H13" s="26">
+        <f>H2*'Budgetierte Kosten'!$Q2</f>
+        <v>8.6400000000000005E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="str">
+        <f>'Budgetierte Kosten'!A3</f>
+        <v>Design und Architektur</v>
+      </c>
+      <c r="B14" s="26">
+        <f>B3*'Budgetierte Kosten'!$Q3</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="26">
+        <f>C3*'Budgetierte Kosten'!$Q3</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="26">
+        <f>D3*'Budgetierte Kosten'!$Q3</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="26">
+        <f>E3*'Budgetierte Kosten'!$Q3</f>
+        <v>7.8666666666666659E-3</v>
+      </c>
+      <c r="F14" s="26">
+        <f>F3*'Budgetierte Kosten'!$Q3</f>
+        <v>7.8666666666666659E-3</v>
+      </c>
+      <c r="G14" s="26">
+        <f>G3*'Budgetierte Kosten'!$Q3</f>
+        <v>1.5733333333333332E-2</v>
+      </c>
+      <c r="H14" s="26">
+        <f>H3*'Budgetierte Kosten'!$Q3</f>
+        <v>6.2933333333333327E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="str">
+        <f>'Budgetierte Kosten'!A4</f>
+        <v>Implementierung</v>
+      </c>
+      <c r="B15" s="26">
+        <f>B4*'Budgetierte Kosten'!$Q4</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="26">
+        <f>C4*'Budgetierte Kosten'!$Q4</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="26">
+        <f>D4*'Budgetierte Kosten'!$Q4</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="26">
+        <f>E4*'Budgetierte Kosten'!$Q4</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="26">
+        <f>F4*'Budgetierte Kosten'!$Q4</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="26">
+        <f>G4*'Budgetierte Kosten'!$Q4</f>
+        <v>2.6133333333333331E-2</v>
+      </c>
+      <c r="H15" s="26">
+        <f>H4*'Budgetierte Kosten'!$Q4</f>
+        <v>6.5333333333333327E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="str">
+        <f>'Budgetierte Kosten'!A5</f>
+        <v>Integration und Test</v>
+      </c>
+      <c r="B16" s="26">
+        <f>B5*'Budgetierte Kosten'!$Q5</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="26">
+        <f>C5*'Budgetierte Kosten'!$Q5</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="26">
+        <f>D5*'Budgetierte Kosten'!$Q5</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="26">
+        <f>E5*'Budgetierte Kosten'!$Q5</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="26">
+        <f>F5*'Budgetierte Kosten'!$Q5</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="26">
+        <f>G5*'Budgetierte Kosten'!$Q5</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="26">
+        <f>H5*'Budgetierte Kosten'!$Q5</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="str">
+        <f>'Budgetierte Kosten'!A6</f>
+        <v>Projektmanagement</v>
+      </c>
+      <c r="B17" s="26">
+        <f>B6*'Budgetierte Kosten'!$Q6</f>
+        <v>1.5253333333333334E-2</v>
+      </c>
+      <c r="C17" s="26">
+        <f>C6*'Budgetierte Kosten'!$Q6</f>
+        <v>9.5333333333333346E-3</v>
+      </c>
+      <c r="D17" s="26">
+        <f>D6*'Budgetierte Kosten'!$Q6</f>
+        <v>2.86E-2</v>
+      </c>
+      <c r="E17" s="26">
+        <f>E6*'Budgetierte Kosten'!$Q6</f>
+        <v>3.8133333333333339E-2</v>
+      </c>
+      <c r="F17" s="26">
+        <f>F6*'Budgetierte Kosten'!$Q6</f>
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="G17" s="26">
+        <f>G6*'Budgetierte Kosten'!$Q6</f>
+        <v>7.6266666666666677E-2</v>
+      </c>
+      <c r="H17" s="26">
+        <f>H6*'Budgetierte Kosten'!$Q6</f>
+        <v>9.5333333333333339E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="str">
+        <f>'Budgetierte Kosten'!A7</f>
+        <v>Puffer für unerwartetes</v>
+      </c>
+      <c r="B18" s="26">
+        <f>B7*'Budgetierte Kosten'!$Q7</f>
+        <v>5.5466666666666668E-3</v>
+      </c>
+      <c r="C18" s="26">
+        <f>C7*'Budgetierte Kosten'!$Q7</f>
+        <v>3.4666666666666665E-3</v>
+      </c>
+      <c r="D18" s="26">
+        <f>D7*'Budgetierte Kosten'!$Q7</f>
+        <v>6.933333333333333E-3</v>
+      </c>
+      <c r="E18" s="26">
+        <f>E7*'Budgetierte Kosten'!$Q7</f>
+        <v>1.3866666666666666E-2</v>
+      </c>
+      <c r="F18" s="26">
+        <f>F7*'Budgetierte Kosten'!$Q7</f>
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="G18" s="26">
+        <f>G7*'Budgetierte Kosten'!$Q7</f>
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="H18" s="26">
+        <f>H7*'Budgetierte Kosten'!$Q7</f>
+        <v>3.8133333333333332E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="26">
+        <f>B8*'Budgetierte Kosten'!$Q11</f>
+        <v>1.1466666666666667E-3</v>
+      </c>
+      <c r="C19" s="26">
+        <f>C8*'Budgetierte Kosten'!$Q11</f>
+        <v>2.2933333333333334E-3</v>
+      </c>
+      <c r="D19" s="26">
+        <f>D8*'Budgetierte Kosten'!$Q11</f>
+        <v>3.4399999999999999E-3</v>
+      </c>
+      <c r="E19" s="26">
+        <f>E8*'Budgetierte Kosten'!$Q11</f>
+        <v>4.5866666666666668E-3</v>
+      </c>
+      <c r="F19" s="26">
+        <f>F8*'Budgetierte Kosten'!$Q11</f>
+        <v>5.7333333333333333E-3</v>
+      </c>
+      <c r="G19" s="26">
+        <f>G8*'Budgetierte Kosten'!$Q11</f>
+        <v>6.8799999999999998E-3</v>
+      </c>
+      <c r="H19" s="26">
+        <f>H8*'Budgetierte Kosten'!$Q11</f>
+        <v>8.0266666666666681E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="B20" s="17">
+        <f>SUM(B13:B19)</f>
+        <v>5.5546666666666661E-2</v>
+      </c>
+      <c r="C20" s="17">
+        <f t="shared" ref="C20:H20" si="0">SUM(C13:C19)</f>
+        <v>2.0093333333333338E-2</v>
+      </c>
+      <c r="D20" s="17">
+        <f t="shared" si="0"/>
+        <v>4.8573333333333329E-2</v>
+      </c>
+      <c r="E20" s="17">
+        <f t="shared" si="0"/>
+        <v>9.3253333333333341E-2</v>
+      </c>
+      <c r="F20" s="17">
+        <f t="shared" si="0"/>
+        <v>0.13960000000000003</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" si="0"/>
+        <v>0.23301333333333335</v>
+      </c>
+      <c r="H20" s="17">
+        <f t="shared" si="0"/>
+        <v>0.39816000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
raw entwurf management bericht
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
@@ -617,10 +617,39 @@
   </cellStyles>
   <dxfs count="126">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <fill>
@@ -663,35 +692,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -42152,20 +42152,20 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="16">
+    <tableColumn id="2" name="CPI" dataDxfId="10">
       <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="15">
+    <tableColumn id="3" name="SPI" dataDxfId="9">
       <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="1">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="14"/>
-    <tableColumn id="6" name="Status" dataDxfId="13">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="7"/>
+    <tableColumn id="6" name="Status" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Trend" dataDxfId="12">
+    <tableColumn id="7" name="Trend" dataDxfId="5">
       <calculatedColumnFormula>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -42180,19 +42180,19 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="11">
+    <tableColumn id="2" name="CPI" dataDxfId="4">
       <calculatedColumnFormula>Kennzahlen!H69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="10">
+    <tableColumn id="3" name="SPI" dataDxfId="3">
       <calculatedColumnFormula>Kennzahlen!H82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="0">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="2">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="9">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="1">
       <calculatedColumnFormula>F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Status" dataDxfId="8">
+    <tableColumn id="6" name="Status" dataDxfId="0">
       <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Trend"/>
@@ -42909,7 +42909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L119" sqref="L119"/>
     </sheetView>
   </sheetViews>
@@ -46069,7 +46069,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46091,7 +46091,7 @@
         <v>48</v>
       </c>
       <c r="K3">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -46146,7 +46146,7 @@
       </c>
       <c r="G5" s="32" t="str">
         <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
-        <v>Gelb</v>
+        <v>Rot</v>
       </c>
       <c r="H5" t="str">
         <f>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</f>
@@ -46176,7 +46176,7 @@
       </c>
       <c r="G6" s="32" t="str">
         <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
-        <v>Gelb</v>
+        <v>Rot</v>
       </c>
       <c r="H6" t="str">
         <f>IF(C19=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C19)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C19,Tabelle9[[#This Row],[SPI]]&lt;D19), $K$11, $K$10)))</f>
@@ -46212,7 +46212,7 @@
       </c>
       <c r="G7" s="32" t="str">
         <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
-        <v>Gelb</v>
+        <v>Rot</v>
       </c>
       <c r="H7" t="str">
         <f>IF(C20=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C20)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C20,Tabelle9[[#This Row],[SPI]]&lt;D20), $K$11, $K$10)))</f>
@@ -46284,7 +46284,7 @@
       </c>
       <c r="G9" s="32" t="str">
         <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
-        <v>Gelb</v>
+        <v>Rot</v>
       </c>
       <c r="H9" t="str">
         <f>IF(C22=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C22)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C22,Tabelle9[[#This Row],[SPI]]&lt;D22), $K$11, $K$10)))</f>
@@ -46350,7 +46350,7 @@
       </c>
       <c r="G11" s="32" t="str">
         <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
-        <v>Gelb</v>
+        <v>Rot</v>
       </c>
       <c r="H11" t="str">
         <f>IF(C24=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C24)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C24,Tabelle9[[#This Row],[SPI]]&lt;D24), $K$11, $K$10)))</f>
@@ -46386,7 +46386,7 @@
       </c>
       <c r="G12" s="34" t="str">
         <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
-        <v>Gelb</v>
+        <v>Rot</v>
       </c>
       <c r="H12" s="35" t="str">
         <f>IF(C25=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C25)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C25,Tabelle9[[#This Row],[SPI]]&lt;D25), $K$11, $K$10)))</f>
@@ -46458,7 +46458,7 @@
       </c>
       <c r="G18" s="32" t="str">
         <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
-        <v>Gelb</v>
+        <v>Rot</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
@@ -46562,7 +46562,7 @@
       </c>
       <c r="G22" s="32" t="str">
         <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
-        <v>Gelb</v>
+        <v>Rot</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
@@ -46614,7 +46614,7 @@
       </c>
       <c r="G24" s="32" t="str">
         <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
-        <v>Gelb</v>
+        <v>Rot</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
@@ -46645,13 +46645,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D12 C18:D25">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThanOrEqual">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>$K$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
some changes i forgot to commit yesterday :*
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="90">
   <si>
     <t>Aktivität / Monat</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>Fertigstellungsgrad in Relation zum beigetragenen BAC</t>
+  </si>
+  <si>
+    <t>Test:</t>
   </si>
 </sst>
 </file>
@@ -617,41 +620,6 @@
   </cellStyles>
   <dxfs count="126">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF6969"/>
@@ -692,6 +660,41 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -42152,20 +42155,20 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="10">
+    <tableColumn id="2" name="CPI" dataDxfId="16">
       <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="9">
+    <tableColumn id="3" name="SPI" dataDxfId="15">
       <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="14">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="7"/>
-    <tableColumn id="6" name="Status" dataDxfId="6">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="13"/>
+    <tableColumn id="6" name="Status" dataDxfId="12">
       <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Trend" dataDxfId="5">
+    <tableColumn id="7" name="Trend" dataDxfId="11">
       <calculatedColumnFormula>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -42180,19 +42183,19 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="4">
+    <tableColumn id="2" name="CPI" dataDxfId="10">
       <calculatedColumnFormula>Kennzahlen!H69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="3">
+    <tableColumn id="3" name="SPI" dataDxfId="9">
       <calculatedColumnFormula>Kennzahlen!H82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="2">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="1">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="7">
       <calculatedColumnFormula>F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Status" dataDxfId="0">
+    <tableColumn id="6" name="Status" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Trend"/>
@@ -42909,8 +42912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N97" sqref="N97"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -43250,7 +43253,10 @@
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
-      <c r="K13">
+      <c r="K13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L13">
         <f>SUM(PV[7])</f>
         <v>723000</v>
       </c>
@@ -43563,13 +43569,19 @@
         <f>SUM('Tatsächliche Kosten'!$B12:'Tatsächliche Kosten'!H12)</f>
         <v>868750</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L24">
         <f>SUM(AC[1])</f>
         <v>83600</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K25">
+      <c r="K25" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L25">
         <f>SUM(AC[7])</f>
         <v>868750</v>
       </c>
@@ -44236,13 +44248,19 @@
         <f>EV[[#Totals],[7]]-AC[[#Totals],[7]]</f>
         <v>-271510</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L50">
         <f>SUM(CV[1])</f>
         <v>-280</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K51">
+      <c r="K51" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L51">
         <f>SUM(CV[7])</f>
         <v>-271510</v>
       </c>
@@ -44521,7 +44539,10 @@
         <f t="shared" si="5"/>
         <v>-8959.9999999999982</v>
       </c>
-      <c r="K62">
+      <c r="K62" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L62">
         <f>SUM(SV[1])</f>
         <v>3320</v>
       </c>
@@ -44559,7 +44580,10 @@
         <f>SUM(SV[7])</f>
         <v>-125760</v>
       </c>
-      <c r="K63">
+      <c r="K63" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L63">
         <f>SUM(SV[7])</f>
         <v>-125760</v>
       </c>
@@ -45252,6 +45276,11 @@
         <v>67</v>
       </c>
     </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N95" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>16</v>
@@ -45681,6 +45710,9 @@
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K106" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="L106">
         <f>SUM(ETC[7 '[k €']])</f>
         <v>955.91504329004329</v>
@@ -45993,6 +46025,9 @@
       <c r="I117" s="29">
         <f>$E$92/(CPI[[#Totals],[7]]*1000)</f>
         <v>2181.9117942535663</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="L117">
         <f>I110*I69</f>
@@ -46645,13 +46680,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D12 C18:D25">
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="greaterThanOrEqual">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="lessThan">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="lessThan">
       <formula>$K$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46710,8 +46745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O170" sqref="O170"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -48323,7 +48358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Szenario geschrieben, wie es zu dem Projektverlauf kam, Bilder eingefügt, Budget der RAG Gesamtzeile verändert, Farben der Diagramme mit CV/SV verändert/vertauscht - SV hatte dieselbe Farbe wie AC, CV dieselbe wie PV, vermittelte faelschlichen Zusammenhang
</commit_message>
<xml_diff>
--- a/Lab1/Erster Entwurf Christian.xlsx
+++ b/Lab1/Erster Entwurf Christian.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
@@ -620,6 +620,41 @@
   </cellStyles>
   <dxfs count="126">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF6969"/>
@@ -660,41 +695,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -12878,7 +12878,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -12893,7 +12893,9 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -12982,7 +12984,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -12997,7 +12999,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -13526,7 +13528,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -13541,7 +13543,9 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -13630,7 +13634,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -13645,7 +13649,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -14174,7 +14178,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -14189,7 +14193,9 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -14278,7 +14284,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -14293,7 +14299,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -14822,7 +14828,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -14837,12 +14843,38 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:symbol val="x"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-5FFF-47CD-BEA3-6421FCB16B9E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:xVal>
             <c:strRef>
               <c:f>Kennzahlen!$C$3:$I$3</c:f>
@@ -14926,7 +14958,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -14941,7 +14973,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -16112,7 +16144,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -16127,7 +16159,9 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -16216,7 +16250,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -16231,7 +16265,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -16760,7 +16794,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -16775,7 +16809,9 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -16864,7 +16900,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -16879,7 +16915,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -17408,7 +17444,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -17423,7 +17459,9 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -17512,7 +17550,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -17527,7 +17565,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -18056,7 +18094,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -18071,7 +18109,9 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -18160,7 +18200,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -18175,7 +18215,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -42155,20 +42195,20 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="16">
+    <tableColumn id="2" name="CPI" dataDxfId="10">
       <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="15">
+    <tableColumn id="3" name="SPI" dataDxfId="9">
       <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="14">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="13"/>
-    <tableColumn id="6" name="Status" dataDxfId="12">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="7"/>
+    <tableColumn id="6" name="Status" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Trend" dataDxfId="11">
+    <tableColumn id="7" name="Trend" dataDxfId="5">
       <calculatedColumnFormula>IF(C18=Kennzahlen!$L$70,Kennzahlen!$L$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -42183,19 +42223,19 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="10">
+    <tableColumn id="2" name="CPI" dataDxfId="4">
       <calculatedColumnFormula>Kennzahlen!H69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="9">
+    <tableColumn id="3" name="SPI" dataDxfId="3">
       <calculatedColumnFormula>Kennzahlen!H82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="2">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="7">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="1">
       <calculatedColumnFormula>F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Status" dataDxfId="6">
+    <tableColumn id="6" name="Status" dataDxfId="0">
       <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Trend"/>
@@ -42912,7 +42952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -46103,8 +46143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46416,8 +46456,7 @@
         <v>0.39816000000000001</v>
       </c>
       <c r="F12" s="31">
-        <f>'Budgetierte Kosten'!P11/1000</f>
-        <v>1500</v>
+        <v>1250</v>
       </c>
       <c r="G12" s="34" t="str">
         <f>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
@@ -46671,7 +46710,7 @@
       </c>
       <c r="F25" s="31">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1250</v>
       </c>
       <c r="G25" s="34" t="str">
         <f>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</f>
@@ -46680,13 +46719,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D12 C18:D25">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThanOrEqual">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>$K$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46745,8 +46784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView showGridLines="0" topLeftCell="U119" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE162" sqref="AE162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46761,7 +46800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>

</xml_diff>